<commit_message>
Agrego casos de prueba
</commit_message>
<xml_diff>
--- a/ISW_Grupo6_4k2/Practicos/TP12/Resolucion_12_TestionMetodosCajaNegra.xlsx
+++ b/ISW_Grupo6_4k2/Practicos/TP12/Resolucion_12_TestionMetodosCajaNegra.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tamara\Documents\UTN\4toaño\ISW\Repo\ISW_Grupo6_4K2\ISW_Grupo6_4k2\Practicos\TP12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F293AF-2338-4015-B2AB-E43C23756592}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A791F7F3-ACF3-4DB8-ACBD-6BF1C3902DCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="679" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos_Prueba" sheetId="27" r:id="rId1"/>
@@ -24,13 +24,13 @@
     <definedName name="Ready_To_Run" localSheetId="0">#REF!</definedName>
     <definedName name="Ready_To_Run">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="179021"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="134">
   <si>
     <t>TC_001</t>
   </si>
@@ -338,9 +338,6 @@
     <t>Sin foto</t>
   </si>
   <si>
-    <t>Foto con tamaño &gt;= 5Mb</t>
-  </si>
-  <si>
     <t>Foto con formato distinto a JPG</t>
   </si>
   <si>
@@ -387,6 +384,54 @@
   </si>
   <si>
     <t>"Mensajes de error"</t>
+  </si>
+  <si>
+    <t>Foto con tamaño &gt; 5Mb</t>
+  </si>
+  <si>
+    <t>Realizar pedido "Lo que sea" en efectivo, lo antes posibe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Usuario logueado </t>
+  </si>
+  <si>
+    <t>1, 5, 7, 10, 15</t>
+  </si>
+  <si>
+    <t>Se muestra mensaje de confirmacion "Pedido realizado exitosamente"</t>
+  </si>
+  <si>
+    <t>Realizar pedido "Lo que sea" en tarjeta, lo antes posibe</t>
+  </si>
+  <si>
+    <t>Usuario logueado</t>
+  </si>
+  <si>
+    <t>Realizar pedido "Lo que sea" programando fecha y hora de entrega</t>
+  </si>
+  <si>
+    <t>Realizar pedido "Lo que sea" con tarjeta invalida</t>
+  </si>
+  <si>
+    <t>1- Se selecciona opcion "Realizar nuevo pedido"   2-  Se ingresa "Cerveza andes" como pedido      3- No se adjunta foto                                                   4- Se ingresa usando mapa de google la ubicación del comercio                                               5- Se ingresa la direccion de entrega "A. Sanchez ariño 2505"                                                                  6- Se ingresa forma de pago "TARJETA 0021215545612"                 7- Se ingresa recibirlo "LO ANTES POSIBLE"               8- Se confirma pedido.</t>
+  </si>
+  <si>
+    <t>Se muestra mensaje "El número de tarjeta es invalido, ingrese numero valido"</t>
+  </si>
+  <si>
+    <t>1, 5, 7, 12, 15</t>
+  </si>
+  <si>
+    <t>1- Se selecciona opcion "Realizar nuevo pedido"   2-  Se ingresa "Cerveza andes" como pedido      3- No se adjunta foto                                                   4- Se ingresa usando mapa de google la ubicación del comercio                                               5- Se ingresa la direccion de entrega "A. Sanchez ariño 2505"                                                                  6- Se ingresa forma de pago "EFECTIVO"                    7- Se ingresa $150 como monto a pagar                   8- Se ingresa recibirlo "LO ANTES POSIBLE"               9- Se confirma pedido.</t>
+  </si>
+  <si>
+    <t>Realizar pedido "Lo que sea" con fecha de entrega invalida</t>
+  </si>
+  <si>
+    <t>1- Se selecciona opcion "Realizar nuevo pedido"   2-  Se ingresa "Cerveza andes" como pedido      3- No se adjunta foto                                                   4- Se ingresa usando mapa de google la ubicación del comercio                                               5- Se ingresa la direccion de entrega "A. Sanchez ariño 2505"                                                                  6- Se ingresa forma de pago "TARJETA 0021215545612"                 7- Se ingresa recibirlo "El dia 14/10/2015"               8- Se confirma pedido.</t>
+  </si>
+  <si>
+    <t>Se muestra mensaje "La fecha ingresada debe ser mayor a la fecha actual"</t>
   </si>
 </sst>
 </file>
@@ -890,7 +935,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -996,6 +1041,14 @@
     <xf numFmtId="14" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="14" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1020,38 +1073,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1072,6 +1102,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1866,9 +1918,9 @@
   </sheetPr>
   <dimension ref="A1:AS73"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1931,14 +1983,14 @@
       <c r="AE1" s="4"/>
     </row>
     <row r="2" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
       <c r="G2" s="32"/>
       <c r="H2" s="32"/>
       <c r="I2" s="32"/>
@@ -1966,12 +2018,12 @@
       <c r="AE2" s="4"/>
     </row>
     <row r="3" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
       <c r="G3" s="32"/>
       <c r="H3" s="32"/>
       <c r="I3" s="32"/>
@@ -1999,12 +2051,12 @@
       <c r="AE3" s="4"/>
     </row>
     <row r="4" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
+      <c r="A4" s="53"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
       <c r="G4" s="32"/>
       <c r="H4" s="32"/>
       <c r="I4" s="32"/>
@@ -2032,14 +2084,14 @@
       <c r="AE4" s="4"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="47"/>
+      <c r="B5" s="55"/>
       <c r="C5" s="43"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="59"/>
       <c r="G5" s="33"/>
       <c r="H5" s="33"/>
       <c r="I5" s="33"/>
@@ -2093,34 +2145,34 @@
     </row>
     <row r="7" spans="1:45" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:45" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="48"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="46" t="s">
+      <c r="A8" s="56"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46" t="s">
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="N8" s="46"/>
-      <c r="O8" s="46"/>
-      <c r="P8" s="46"/>
-      <c r="Q8" s="46"/>
-      <c r="R8" s="46" t="s">
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="S8" s="46"/>
-      <c r="T8" s="46"/>
-      <c r="U8" s="46"/>
-      <c r="V8" s="46"/>
+      <c r="S8" s="54"/>
+      <c r="T8" s="54"/>
+      <c r="U8" s="54"/>
+      <c r="V8" s="54"/>
     </row>
     <row r="9" spans="1:45" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
@@ -2218,16 +2270,26 @@
       <c r="AB10" s="6"/>
       <c r="AL10" s="6"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" ht="132" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="77" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>122</v>
+      </c>
       <c r="H11" s="26"/>
       <c r="I11" s="15"/>
       <c r="J11" s="29"/>
@@ -2250,14 +2312,18 @@
       <c r="AR11" s="7"/>
       <c r="AS11" s="7"/>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" ht="24" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="26"/>
+      <c r="D12" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>124</v>
+      </c>
       <c r="F12" s="26"/>
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
@@ -2282,13 +2348,15 @@
       <c r="AR12" s="7"/>
       <c r="AS12" s="7"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" ht="24" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
+      <c r="D13" s="21" t="s">
+        <v>125</v>
+      </c>
       <c r="E13" s="26"/>
       <c r="F13" s="26"/>
       <c r="G13" s="26"/>
@@ -2314,16 +2382,26 @@
       <c r="AR13" s="7"/>
       <c r="AS13" s="7"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" ht="132" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
+      <c r="C14" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>128</v>
+      </c>
       <c r="H14" s="26"/>
       <c r="I14" s="15"/>
       <c r="J14" s="28"/>
@@ -2346,16 +2424,24 @@
       <c r="AR14" s="7"/>
       <c r="AS14" s="7"/>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45" ht="132" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
+      <c r="D15" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>133</v>
+      </c>
       <c r="H15" s="26"/>
       <c r="I15" s="15"/>
       <c r="J15" s="28"/>
@@ -4433,989 +4519,980 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724181F4-A37D-478F-88A3-A3E54FC7D574}">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="55.140625" customWidth="1"/>
-    <col min="8" max="8" width="31" customWidth="1"/>
+    <col min="8" max="8" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="75"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="70"/>
     </row>
     <row r="2" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="64" t="s">
+      <c r="B2" s="74"/>
+      <c r="C2" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="55" t="s">
+      <c r="D2" s="75"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="73" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="58"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="46"/>
     </row>
     <row r="3" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="75"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="70"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="53">
+      <c r="B4" s="65"/>
+      <c r="C4" s="76">
         <v>1</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="52"/>
-      <c r="F4" s="53">
+      <c r="E4" s="63"/>
+      <c r="F4" s="76">
         <v>3</v>
       </c>
-      <c r="G4" s="52" t="s">
+      <c r="G4" s="61" t="s">
         <v>94</v>
       </c>
-      <c r="H4" s="52"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="58"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="46"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="71"/>
-      <c r="B5" s="72"/>
-      <c r="C5" s="53">
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="47">
         <v>2</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="53">
+      <c r="E5" s="72"/>
+      <c r="F5" s="47">
         <v>4</v>
       </c>
-      <c r="G5" s="52" t="s">
+      <c r="G5" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="H5" s="52"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="58"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="46"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="60"/>
-      <c r="B6" s="58"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="58"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="46"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="53">
+      <c r="B7" s="72"/>
+      <c r="C7" s="47">
         <v>5</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="D7" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="53">
+      <c r="E7" s="72"/>
+      <c r="F7" s="47">
         <v>6</v>
       </c>
-      <c r="G7" s="52" t="s">
+      <c r="G7" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="58"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="46"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="60"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="58"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="46"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="71" t="s">
+      <c r="A9" s="66" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="53">
+      <c r="B9" s="67"/>
+      <c r="C9" s="47">
         <v>6</v>
       </c>
-      <c r="D9" s="52" t="s">
+      <c r="D9" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="52"/>
-      <c r="F9" s="53">
+      <c r="E9" s="72"/>
+      <c r="F9" s="47">
         <v>8</v>
       </c>
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="H9" s="72"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="46"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="66"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="47">
+        <v>7</v>
+      </c>
+      <c r="D10" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" s="72"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="H10" s="72"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="46"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="47"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="46"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="66" t="s">
         <v>103</v>
       </c>
-      <c r="H9" s="52"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="58"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="71"/>
-      <c r="B10" s="72"/>
-      <c r="C10" s="53">
-        <v>7</v>
-      </c>
-      <c r="D10" s="52" t="s">
-        <v>101</v>
-      </c>
-      <c r="E10" s="52"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="52" t="s">
-        <v>102</v>
-      </c>
-      <c r="H10" s="52"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="58"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="60"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="58"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="71" t="s">
+      <c r="B12" s="67"/>
+      <c r="C12" s="47">
+        <v>9</v>
+      </c>
+      <c r="D12" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="E12" s="72"/>
+      <c r="F12" s="47">
+        <v>11</v>
+      </c>
+      <c r="G12" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="B12" s="72"/>
-      <c r="C12" s="53">
-        <v>9</v>
-      </c>
-      <c r="D12" s="52" t="s">
+      <c r="H12" s="72"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="46"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="66"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="47">
+        <v>10</v>
+      </c>
+      <c r="D13" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="E12" s="52"/>
-      <c r="F12" s="53">
-        <v>11</v>
-      </c>
-      <c r="G12" s="52" t="s">
-        <v>105</v>
-      </c>
-      <c r="H12" s="52"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="58"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="71"/>
-      <c r="B13" s="72"/>
-      <c r="C13" s="53">
-        <v>10</v>
-      </c>
-      <c r="D13" s="52" t="s">
+      <c r="E13" s="72"/>
+      <c r="F13" s="47">
+        <v>12</v>
+      </c>
+      <c r="G13" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="E13" s="52"/>
-      <c r="F13" s="53">
-        <v>12</v>
-      </c>
-      <c r="G13" s="52" t="s">
+      <c r="H13" s="72"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="46"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="47"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="47">
+        <v>13</v>
+      </c>
+      <c r="G14" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="H13" s="52"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="58"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="60"/>
-      <c r="B14" s="58"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="53">
-        <v>13</v>
-      </c>
-      <c r="G14" s="52" t="s">
+      <c r="H14" s="72"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="46"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="47"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="72"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="46"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="H14" s="52"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="58"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="60"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="53">
+      <c r="B16" s="67"/>
+      <c r="C16" s="47">
+        <v>14</v>
+      </c>
+      <c r="D16" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" s="72"/>
+      <c r="F16" s="47">
         <v>16</v>
       </c>
-      <c r="G15" s="52" t="s">
+      <c r="G16" s="60" t="s">
+        <v>112</v>
+      </c>
+      <c r="H16" s="72"/>
+      <c r="L16" s="45"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="66"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="47">
+        <v>15</v>
+      </c>
+      <c r="D17" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="72"/>
+      <c r="F17" s="47">
+        <v>17</v>
+      </c>
+      <c r="G17" s="60" t="s">
         <v>113</v>
       </c>
-      <c r="H15" s="52"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="58"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="71" t="s">
-        <v>110</v>
-      </c>
-      <c r="B16" s="72"/>
-      <c r="C16" s="53">
-        <v>14</v>
-      </c>
-      <c r="D16" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="E16" s="52"/>
-      <c r="F16" s="53">
-        <v>17</v>
-      </c>
-      <c r="G16" s="52" t="s">
+      <c r="H17" s="72"/>
+      <c r="I17" s="45"/>
+      <c r="L17" s="45"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="47"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="46"/>
+    </row>
+    <row r="19" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="48"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="46"/>
+    </row>
+    <row r="20" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="H16" s="52"/>
-      <c r="L16" s="53"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="71"/>
-      <c r="B17" s="72"/>
-      <c r="C17" s="53">
-        <v>15</v>
-      </c>
-      <c r="D17" s="52" t="s">
-        <v>112</v>
-      </c>
-      <c r="E17" s="52"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="53"/>
-      <c r="L17" s="53"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="60"/>
-      <c r="B18" s="58"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="58"/>
-    </row>
-    <row r="19" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="61"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="58"/>
-    </row>
-    <row r="20" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="73" t="s">
+      <c r="B20" s="69"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="69"/>
+      <c r="J20" s="69"/>
+      <c r="K20" s="69"/>
+      <c r="L20" s="70"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="74"/>
-      <c r="C20" s="74"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="74"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="75"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="54" t="s">
+      <c r="B21" s="63"/>
+      <c r="C21" s="76">
+        <v>18</v>
+      </c>
+      <c r="D21" s="61" t="s">
         <v>116</v>
       </c>
-      <c r="B21" s="56"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="55" t="s">
+      <c r="E21" s="63"/>
+      <c r="F21" s="76">
+        <v>19</v>
+      </c>
+      <c r="G21" s="61" t="s">
         <v>117</v>
       </c>
-      <c r="E21" s="55"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="H21" s="55"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="67"/>
-      <c r="K21" s="67"/>
-      <c r="L21" s="68"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="52"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="60"/>
-      <c r="B22" s="58"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="58"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="47">
+        <v>20</v>
+      </c>
+      <c r="G22" s="45"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="46"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="60"/>
-      <c r="B23" s="58"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="53"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="58"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="47">
+        <v>21</v>
+      </c>
+      <c r="G23" s="45"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="46"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="60"/>
-      <c r="B24" s="58"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="58"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="47">
+        <v>22</v>
+      </c>
+      <c r="G24" s="45"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="46"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="60"/>
-      <c r="B25" s="58"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="53"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="58"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="46"/>
     </row>
     <row r="26" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="61"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="62"/>
-      <c r="K26" s="62"/>
-      <c r="L26" s="63"/>
+      <c r="A26" s="48"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="50"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="53"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="53"/>
-      <c r="K27" s="53"/>
-      <c r="L27" s="58"/>
+      <c r="A27" s="45"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="46"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="60"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="53"/>
-      <c r="J28" s="53"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="58"/>
+      <c r="A28" s="47"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="46"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="60"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="53"/>
-      <c r="K29" s="53"/>
-      <c r="L29" s="58"/>
+      <c r="A29" s="47"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="46"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="60"/>
-      <c r="B30" s="53"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="53"/>
-      <c r="L30" s="58"/>
+      <c r="A30" s="47"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="46"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="60"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="53"/>
-      <c r="J31" s="53"/>
-      <c r="K31" s="53"/>
-      <c r="L31" s="58"/>
+      <c r="A31" s="47"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="46"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="60"/>
-      <c r="B32" s="53"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="53"/>
-      <c r="K32" s="53"/>
-      <c r="L32" s="58"/>
+      <c r="A32" s="47"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="46"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="60"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="53"/>
-      <c r="K33" s="53"/>
-      <c r="L33" s="58"/>
+      <c r="A33" s="47"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="46"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="60"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="53"/>
-      <c r="G34" s="53"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="53"/>
-      <c r="J34" s="53"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="58"/>
+      <c r="A34" s="47"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="45"/>
+      <c r="L34" s="46"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="60"/>
-      <c r="B35" s="53"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
-      <c r="G35" s="53"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="53"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="58"/>
+      <c r="A35" s="47"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="45"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="46"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="60"/>
-      <c r="B36" s="53"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="53"/>
-      <c r="I36" s="53"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="53"/>
-      <c r="L36" s="58"/>
+      <c r="A36" s="47"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="45"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="46"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="60"/>
-      <c r="B37" s="53"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
-      <c r="G37" s="53"/>
-      <c r="H37" s="53"/>
-      <c r="I37" s="53"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="58"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="46"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="60"/>
-      <c r="B38" s="53"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="53"/>
-      <c r="G38" s="53"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="58"/>
+      <c r="A38" s="47"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="46"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="60"/>
-      <c r="B39" s="53"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="53"/>
-      <c r="G39" s="53"/>
-      <c r="H39" s="53"/>
-      <c r="I39" s="53"/>
-      <c r="J39" s="53"/>
-      <c r="K39" s="53"/>
-      <c r="L39" s="58"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="45"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="45"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="45"/>
+      <c r="L39" s="46"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="60"/>
-      <c r="B40" s="53"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="53"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="53"/>
-      <c r="G40" s="53"/>
-      <c r="H40" s="53"/>
-      <c r="I40" s="53"/>
-      <c r="J40" s="53"/>
-      <c r="K40" s="53"/>
-      <c r="L40" s="58"/>
+      <c r="A40" s="47"/>
+      <c r="B40" s="45"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="45"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="45"/>
+      <c r="J40" s="45"/>
+      <c r="K40" s="45"/>
+      <c r="L40" s="46"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="60"/>
-      <c r="B41" s="53"/>
-      <c r="C41" s="53"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="53"/>
-      <c r="G41" s="53"/>
-      <c r="H41" s="53"/>
-      <c r="I41" s="53"/>
-      <c r="J41" s="53"/>
-      <c r="K41" s="53"/>
-      <c r="L41" s="58"/>
+      <c r="A41" s="47"/>
+      <c r="B41" s="45"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="45"/>
+      <c r="J41" s="45"/>
+      <c r="K41" s="45"/>
+      <c r="L41" s="46"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="60"/>
-      <c r="B42" s="53"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="53"/>
-      <c r="F42" s="53"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="53"/>
-      <c r="I42" s="53"/>
-      <c r="J42" s="53"/>
-      <c r="K42" s="53"/>
-      <c r="L42" s="58"/>
+      <c r="A42" s="47"/>
+      <c r="B42" s="45"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="45"/>
+      <c r="J42" s="45"/>
+      <c r="K42" s="45"/>
+      <c r="L42" s="46"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="60"/>
-      <c r="B43" s="53"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="53"/>
-      <c r="F43" s="53"/>
-      <c r="G43" s="53"/>
-      <c r="H43" s="53"/>
-      <c r="I43" s="53"/>
-      <c r="J43" s="53"/>
-      <c r="K43" s="53"/>
-      <c r="L43" s="58"/>
+      <c r="A43" s="47"/>
+      <c r="B43" s="45"/>
+      <c r="C43" s="45"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45"/>
+      <c r="J43" s="45"/>
+      <c r="K43" s="45"/>
+      <c r="L43" s="46"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="60"/>
-      <c r="B44" s="53"/>
-      <c r="C44" s="53"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="53"/>
-      <c r="F44" s="53"/>
-      <c r="G44" s="53"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
-      <c r="K44" s="53"/>
-      <c r="L44" s="58"/>
+      <c r="A44" s="47"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
+      <c r="K44" s="45"/>
+      <c r="L44" s="46"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="60"/>
-      <c r="B45" s="53"/>
-      <c r="C45" s="53"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="53"/>
-      <c r="G45" s="53"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
-      <c r="K45" s="53"/>
-      <c r="L45" s="58"/>
+      <c r="A45" s="47"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
+      <c r="K45" s="45"/>
+      <c r="L45" s="46"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="60"/>
-      <c r="B46" s="53"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="53"/>
-      <c r="J46" s="53"/>
-      <c r="K46" s="53"/>
-      <c r="L46" s="58"/>
+      <c r="A46" s="47"/>
+      <c r="B46" s="45"/>
+      <c r="C46" s="45"/>
+      <c r="D46" s="45"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="45"/>
+      <c r="G46" s="45"/>
+      <c r="H46" s="45"/>
+      <c r="I46" s="45"/>
+      <c r="J46" s="45"/>
+      <c r="K46" s="45"/>
+      <c r="L46" s="46"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A47" s="60"/>
-      <c r="B47" s="53"/>
-      <c r="C47" s="53"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="53"/>
-      <c r="G47" s="53"/>
-      <c r="H47" s="53"/>
-      <c r="I47" s="53"/>
-      <c r="J47" s="53"/>
-      <c r="K47" s="53"/>
-      <c r="L47" s="58"/>
+      <c r="A47" s="47"/>
+      <c r="B47" s="45"/>
+      <c r="C47" s="45"/>
+      <c r="D47" s="45"/>
+      <c r="E47" s="45"/>
+      <c r="F47" s="45"/>
+      <c r="G47" s="45"/>
+      <c r="H47" s="45"/>
+      <c r="I47" s="45"/>
+      <c r="J47" s="45"/>
+      <c r="K47" s="45"/>
+      <c r="L47" s="46"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A48" s="60"/>
-      <c r="B48" s="53"/>
-      <c r="C48" s="53"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="53"/>
-      <c r="F48" s="53"/>
-      <c r="G48" s="53"/>
-      <c r="H48" s="53"/>
-      <c r="I48" s="53"/>
-      <c r="J48" s="53"/>
-      <c r="K48" s="53"/>
-      <c r="L48" s="58"/>
+      <c r="A48" s="47"/>
+      <c r="B48" s="45"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="45"/>
+      <c r="J48" s="45"/>
+      <c r="K48" s="45"/>
+      <c r="L48" s="46"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A49" s="60"/>
-      <c r="B49" s="53"/>
-      <c r="C49" s="53"/>
-      <c r="D49" s="53"/>
-      <c r="E49" s="53"/>
-      <c r="F49" s="53"/>
-      <c r="G49" s="53"/>
-      <c r="H49" s="53"/>
-      <c r="I49" s="53"/>
-      <c r="J49" s="53"/>
-      <c r="K49" s="53"/>
-      <c r="L49" s="58"/>
+      <c r="A49" s="47"/>
+      <c r="B49" s="45"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="45"/>
+      <c r="G49" s="45"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="45"/>
+      <c r="K49" s="45"/>
+      <c r="L49" s="46"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A50" s="60"/>
-      <c r="B50" s="53"/>
-      <c r="C50" s="53"/>
-      <c r="D50" s="53"/>
-      <c r="E50" s="53"/>
-      <c r="F50" s="53"/>
-      <c r="G50" s="53"/>
-      <c r="H50" s="53"/>
-      <c r="I50" s="53"/>
-      <c r="J50" s="53"/>
-      <c r="K50" s="53"/>
-      <c r="L50" s="58"/>
+      <c r="A50" s="47"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="45"/>
+      <c r="K50" s="45"/>
+      <c r="L50" s="46"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A51" s="60"/>
-      <c r="B51" s="53"/>
-      <c r="C51" s="53"/>
-      <c r="D51" s="53"/>
-      <c r="E51" s="53"/>
-      <c r="F51" s="53"/>
-      <c r="G51" s="53"/>
-      <c r="H51" s="53"/>
-      <c r="I51" s="53"/>
-      <c r="J51" s="53"/>
-      <c r="K51" s="53"/>
-      <c r="L51" s="58"/>
+      <c r="A51" s="47"/>
+      <c r="B51" s="45"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="45"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="45"/>
+      <c r="G51" s="45"/>
+      <c r="H51" s="45"/>
+      <c r="I51" s="45"/>
+      <c r="J51" s="45"/>
+      <c r="K51" s="45"/>
+      <c r="L51" s="46"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A52" s="60"/>
-      <c r="B52" s="53"/>
-      <c r="C52" s="53"/>
-      <c r="D52" s="53"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="53"/>
-      <c r="H52" s="53"/>
-      <c r="I52" s="53"/>
-      <c r="J52" s="53"/>
-      <c r="K52" s="53"/>
-      <c r="L52" s="58"/>
+      <c r="A52" s="47"/>
+      <c r="B52" s="45"/>
+      <c r="C52" s="45"/>
+      <c r="D52" s="45"/>
+      <c r="E52" s="45"/>
+      <c r="F52" s="45"/>
+      <c r="G52" s="45"/>
+      <c r="H52" s="45"/>
+      <c r="I52" s="45"/>
+      <c r="J52" s="45"/>
+      <c r="K52" s="45"/>
+      <c r="L52" s="46"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A53" s="60"/>
-      <c r="B53" s="53"/>
-      <c r="C53" s="53"/>
-      <c r="D53" s="53"/>
-      <c r="E53" s="53"/>
-      <c r="F53" s="53"/>
-      <c r="G53" s="53"/>
-      <c r="H53" s="53"/>
-      <c r="I53" s="53"/>
-      <c r="J53" s="53"/>
-      <c r="K53" s="53"/>
-      <c r="L53" s="58"/>
+      <c r="A53" s="47"/>
+      <c r="B53" s="45"/>
+      <c r="C53" s="45"/>
+      <c r="D53" s="45"/>
+      <c r="E53" s="45"/>
+      <c r="F53" s="45"/>
+      <c r="G53" s="45"/>
+      <c r="H53" s="45"/>
+      <c r="I53" s="45"/>
+      <c r="J53" s="45"/>
+      <c r="K53" s="45"/>
+      <c r="L53" s="46"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A54" s="60"/>
-      <c r="B54" s="53"/>
-      <c r="C54" s="53"/>
-      <c r="D54" s="53"/>
-      <c r="E54" s="53"/>
-      <c r="F54" s="53"/>
-      <c r="G54" s="53"/>
-      <c r="H54" s="53"/>
-      <c r="I54" s="53"/>
-      <c r="J54" s="53"/>
-      <c r="K54" s="53"/>
-      <c r="L54" s="58"/>
+      <c r="A54" s="47"/>
+      <c r="B54" s="45"/>
+      <c r="C54" s="45"/>
+      <c r="D54" s="45"/>
+      <c r="E54" s="45"/>
+      <c r="F54" s="45"/>
+      <c r="G54" s="45"/>
+      <c r="H54" s="45"/>
+      <c r="I54" s="45"/>
+      <c r="J54" s="45"/>
+      <c r="K54" s="45"/>
+      <c r="L54" s="46"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A55" s="60"/>
-      <c r="B55" s="53"/>
-      <c r="C55" s="53"/>
-      <c r="D55" s="53"/>
-      <c r="E55" s="53"/>
-      <c r="F55" s="53"/>
-      <c r="G55" s="53"/>
-      <c r="H55" s="53"/>
-      <c r="I55" s="53"/>
-      <c r="J55" s="53"/>
-      <c r="K55" s="53"/>
-      <c r="L55" s="58"/>
+      <c r="A55" s="47"/>
+      <c r="B55" s="45"/>
+      <c r="C55" s="45"/>
+      <c r="D55" s="45"/>
+      <c r="E55" s="45"/>
+      <c r="F55" s="45"/>
+      <c r="G55" s="45"/>
+      <c r="H55" s="45"/>
+      <c r="I55" s="45"/>
+      <c r="J55" s="45"/>
+      <c r="K55" s="45"/>
+      <c r="L55" s="46"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A56" s="60"/>
-      <c r="B56" s="53"/>
-      <c r="C56" s="53"/>
-      <c r="D56" s="53"/>
-      <c r="E56" s="53"/>
-      <c r="F56" s="53"/>
-      <c r="G56" s="53"/>
-      <c r="H56" s="53"/>
-      <c r="I56" s="53"/>
-      <c r="J56" s="53"/>
-      <c r="K56" s="53"/>
-      <c r="L56" s="58"/>
+      <c r="A56" s="47"/>
+      <c r="B56" s="45"/>
+      <c r="C56" s="45"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="45"/>
+      <c r="F56" s="45"/>
+      <c r="G56" s="45"/>
+      <c r="H56" s="45"/>
+      <c r="I56" s="45"/>
+      <c r="J56" s="45"/>
+      <c r="K56" s="45"/>
+      <c r="L56" s="46"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A57" s="60"/>
-      <c r="B57" s="53"/>
-      <c r="C57" s="53"/>
-      <c r="D57" s="53"/>
-      <c r="E57" s="53"/>
-      <c r="F57" s="53"/>
-      <c r="G57" s="53"/>
-      <c r="H57" s="53"/>
-      <c r="I57" s="53"/>
-      <c r="J57" s="53"/>
-      <c r="K57" s="53"/>
-      <c r="L57" s="58"/>
+      <c r="A57" s="47"/>
+      <c r="B57" s="45"/>
+      <c r="C57" s="45"/>
+      <c r="D57" s="45"/>
+      <c r="E57" s="45"/>
+      <c r="F57" s="45"/>
+      <c r="G57" s="45"/>
+      <c r="H57" s="45"/>
+      <c r="I57" s="45"/>
+      <c r="J57" s="45"/>
+      <c r="K57" s="45"/>
+      <c r="L57" s="46"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A58" s="60"/>
-      <c r="B58" s="53"/>
-      <c r="C58" s="53"/>
-      <c r="D58" s="53"/>
-      <c r="E58" s="53"/>
-      <c r="F58" s="53"/>
-      <c r="G58" s="53"/>
-      <c r="H58" s="53"/>
-      <c r="I58" s="53"/>
-      <c r="J58" s="53"/>
-      <c r="K58" s="53"/>
-      <c r="L58" s="58"/>
+      <c r="A58" s="47"/>
+      <c r="B58" s="45"/>
+      <c r="C58" s="45"/>
+      <c r="D58" s="45"/>
+      <c r="E58" s="45"/>
+      <c r="F58" s="45"/>
+      <c r="G58" s="45"/>
+      <c r="H58" s="45"/>
+      <c r="I58" s="45"/>
+      <c r="J58" s="45"/>
+      <c r="K58" s="45"/>
+      <c r="L58" s="46"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A59" s="60"/>
-      <c r="B59" s="53"/>
-      <c r="C59" s="53"/>
-      <c r="D59" s="53"/>
-      <c r="E59" s="53"/>
-      <c r="F59" s="53"/>
-      <c r="G59" s="53"/>
-      <c r="H59" s="53"/>
-      <c r="I59" s="53"/>
-      <c r="J59" s="53"/>
-      <c r="K59" s="53"/>
-      <c r="L59" s="58"/>
+      <c r="A59" s="47"/>
+      <c r="B59" s="45"/>
+      <c r="C59" s="45"/>
+      <c r="D59" s="45"/>
+      <c r="E59" s="45"/>
+      <c r="F59" s="45"/>
+      <c r="G59" s="45"/>
+      <c r="H59" s="45"/>
+      <c r="I59" s="45"/>
+      <c r="J59" s="45"/>
+      <c r="K59" s="45"/>
+      <c r="L59" s="46"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A60" s="60"/>
-      <c r="B60" s="53"/>
-      <c r="C60" s="53"/>
-      <c r="D60" s="53"/>
-      <c r="E60" s="53"/>
-      <c r="F60" s="53"/>
-      <c r="G60" s="53"/>
-      <c r="H60" s="53"/>
-      <c r="I60" s="53"/>
-      <c r="J60" s="53"/>
-      <c r="K60" s="53"/>
-      <c r="L60" s="58"/>
+      <c r="A60" s="47"/>
+      <c r="B60" s="45"/>
+      <c r="C60" s="45"/>
+      <c r="D60" s="45"/>
+      <c r="E60" s="45"/>
+      <c r="F60" s="45"/>
+      <c r="G60" s="45"/>
+      <c r="H60" s="45"/>
+      <c r="I60" s="45"/>
+      <c r="J60" s="45"/>
+      <c r="K60" s="45"/>
+      <c r="L60" s="46"/>
     </row>
     <row r="61" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="61"/>
-      <c r="B61" s="62"/>
-      <c r="C61" s="62"/>
-      <c r="D61" s="62"/>
-      <c r="E61" s="62"/>
-      <c r="F61" s="62"/>
-      <c r="G61" s="62"/>
-      <c r="H61" s="62"/>
-      <c r="I61" s="62"/>
-      <c r="J61" s="62"/>
-      <c r="K61" s="62"/>
-      <c r="L61" s="63"/>
+      <c r="A61" s="48"/>
+      <c r="B61" s="49"/>
+      <c r="C61" s="49"/>
+      <c r="D61" s="49"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="49"/>
+      <c r="G61" s="49"/>
+      <c r="H61" s="49"/>
+      <c r="I61" s="49"/>
+      <c r="J61" s="49"/>
+      <c r="K61" s="49"/>
+      <c r="L61" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A4:B5"/>
-    <mergeCell ref="A9:B10"/>
-    <mergeCell ref="A12:B13"/>
-    <mergeCell ref="A16:B17"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
+  <mergeCells count="41">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
     <mergeCell ref="A20:L20"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="G4:H4"/>
@@ -5432,11 +5509,26 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A4:B5"/>
+    <mergeCell ref="A9:B10"/>
+    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="A16:B17"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G12:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5702,23 +5794,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9EE5A02A2A6DC45B45E782DFEFDA45E" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7657f0a98c495c38e0a3edb0de0bfed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c79c8594d4fa4c9fd200c91a62336472" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -5844,10 +5919,37 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5863,19 +5965,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Agrego mas pruebas TP testing
</commit_message>
<xml_diff>
--- a/ISW_Grupo6_4k2/Practicos/TP12/Resolucion_12_TestionMetodosCajaNegra.xlsx
+++ b/ISW_Grupo6_4k2/Practicos/TP12/Resolucion_12_TestionMetodosCajaNegra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tamara\Documents\UTN\4toaño\ISW\Repo\ISW_Grupo6_4K2\ISW_Grupo6_4k2\Practicos\TP12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A791F7F3-ACF3-4DB8-ACBD-6BF1C3902DCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7112830B-E097-471E-9F6B-D7223581DDD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="144">
   <si>
     <t>TC_001</t>
   </si>
@@ -413,18 +413,12 @@
     <t>Realizar pedido "Lo que sea" con tarjeta invalida</t>
   </si>
   <si>
-    <t>1- Se selecciona opcion "Realizar nuevo pedido"   2-  Se ingresa "Cerveza andes" como pedido      3- No se adjunta foto                                                   4- Se ingresa usando mapa de google la ubicación del comercio                                               5- Se ingresa la direccion de entrega "A. Sanchez ariño 2505"                                                                  6- Se ingresa forma de pago "TARJETA 0021215545612"                 7- Se ingresa recibirlo "LO ANTES POSIBLE"               8- Se confirma pedido.</t>
-  </si>
-  <si>
     <t>Se muestra mensaje "El número de tarjeta es invalido, ingrese numero valido"</t>
   </si>
   <si>
     <t>1, 5, 7, 12, 15</t>
   </si>
   <si>
-    <t>1- Se selecciona opcion "Realizar nuevo pedido"   2-  Se ingresa "Cerveza andes" como pedido      3- No se adjunta foto                                                   4- Se ingresa usando mapa de google la ubicación del comercio                                               5- Se ingresa la direccion de entrega "A. Sanchez ariño 2505"                                                                  6- Se ingresa forma de pago "EFECTIVO"                    7- Se ingresa $150 como monto a pagar                   8- Se ingresa recibirlo "LO ANTES POSIBLE"               9- Se confirma pedido.</t>
-  </si>
-  <si>
     <t>Realizar pedido "Lo que sea" con fecha de entrega invalida</t>
   </si>
   <si>
@@ -432,6 +426,42 @@
   </si>
   <si>
     <t>Se muestra mensaje "La fecha ingresada debe ser mayor a la fecha actual"</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Realizar pedido "Lo que sea" con efectivo sin indicar monto</t>
+  </si>
+  <si>
+    <t>Se visualiza mensaje "Debe ingresar el monto con que va a pagar para continuar con la compra"</t>
+  </si>
+  <si>
+    <t>1, 5, 7, 13, 15</t>
+  </si>
+  <si>
+    <t>Realizar pedido "Lo que sea" sin especificar producto</t>
+  </si>
+  <si>
+    <t>Se visualiza mensaje "Debe ingresar el producto que desea adquirir para efectuar con la compra"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, 6, 7, 10, 15 </t>
+  </si>
+  <si>
+    <t>1- Se selecciona opcion "Realizar nuevo pedido"   2-  Se ingresa "1Kg de helado, sabores chocolate, tramontana, tiramitsu, dulce de leche" como pedido      3- No se adjunta foto                                                   4- Se ingresa usando mapa de google la ubicación del comercio (seleccionando heladeria Gatelin en alta cordoba)                                              5- Se ingresa la direccion de entrega "A. Sanchez ariño 2505"                                                                  6- Se ingresa forma de pago "EFECTIVO"                    7- Se ingresa $400 como monto a pagar                   8- Se ingresa recibirlo "LO ANTES POSIBLE"               9- Se confirma pedido.</t>
+  </si>
+  <si>
+    <t>1- Se selecciona opcion "Realizar nuevo pedido"   Se ingresa "1Kg de helado, sabores chocolate, tramontana, tiramitsu, dulce de leche" como pedido    3- No se adjunta foto                                                   4- Se ingresa usando mapa de google la ubicación del comercio (seleccionando heladeria Gatelin en alta cordoba)                                            5- Se ingresa la direccion de entrega "A. Sanchez ariño 2505"                                                                  6- Se ingresa forma de pago "TARJETA 0021215545612"                 7- Se ingresa recibirlo "LO ANTES POSIBLE"               8- Se confirma pedido.</t>
+  </si>
+  <si>
+    <t>1- Se selecciona opcion "Realizar nuevo pedido"   2-  Se ingresa "Cerveza andes" como pedido      3- No se adjunta foto                                                   4- Se ingresa usando mapa de google la ubicación del comercio (seleccionando heladeria Gatelin en alta cordoba)                                             5- Se ingresa la direccion de entrega "A. Sanchez ariño 2505"                                                                  6- Se ingresa forma de pago "EFECTIVO"                    7- No se ingresa monto a pagar                             8- Se ingresa recibirlo "LO ANTES POSIBLE"               9- Se confirma pedido.</t>
+  </si>
+  <si>
+    <t>1- Se selecciona opcion "Realizar nuevo pedido"   2-  No deja vacio el campo producto solicitado      3- No se adjunta foto                                                   4- Se ingresa usando mapa de google la ubicación del comercio (seleccionando heladeria Gatelin en alta cordoba)                                               5- Se ingresa la direccion de entrega "A. Sanchez ariño 2505"                                                                  6- Se ingresa forma de pago "EFECTIVO"                    7- Se ingresa $400 como monto a pagar                   8- Se ingresa recibirlo "LO ANTES POSIBLE"               9- Se confirma pedido.</t>
   </si>
 </sst>
 </file>
@@ -1049,6 +1079,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="14" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1070,29 +1107,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1109,21 +1131,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1919,8 +1949,8 @@
   <dimension ref="A1:AS73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <pane ySplit="9" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1983,14 +2013,14 @@
       <c r="AE1" s="4"/>
     </row>
     <row r="2" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
       <c r="G2" s="32"/>
       <c r="H2" s="32"/>
       <c r="I2" s="32"/>
@@ -2018,12 +2048,12 @@
       <c r="AE2" s="4"/>
     </row>
     <row r="3" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53"/>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
       <c r="G3" s="32"/>
       <c r="H3" s="32"/>
       <c r="I3" s="32"/>
@@ -2051,12 +2081,12 @@
       <c r="AE3" s="4"/>
     </row>
     <row r="4" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
+      <c r="A4" s="56"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
       <c r="G4" s="32"/>
       <c r="H4" s="32"/>
       <c r="I4" s="32"/>
@@ -2084,14 +2114,14 @@
       <c r="AE4" s="4"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="55"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="43"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="59"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="62"/>
       <c r="G5" s="33"/>
       <c r="H5" s="33"/>
       <c r="I5" s="33"/>
@@ -2145,34 +2175,34 @@
     </row>
     <row r="7" spans="1:45" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:45" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="56"/>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="54" t="s">
+      <c r="A8" s="59"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="54"/>
-      <c r="M8" s="54" t="s">
+      <c r="I8" s="57"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="57"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="N8" s="54"/>
-      <c r="O8" s="54"/>
-      <c r="P8" s="54"/>
-      <c r="Q8" s="54"/>
-      <c r="R8" s="54" t="s">
+      <c r="N8" s="57"/>
+      <c r="O8" s="57"/>
+      <c r="P8" s="57"/>
+      <c r="Q8" s="57"/>
+      <c r="R8" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="S8" s="54"/>
-      <c r="T8" s="54"/>
-      <c r="U8" s="54"/>
-      <c r="V8" s="54"/>
+      <c r="S8" s="57"/>
+      <c r="T8" s="57"/>
+      <c r="U8" s="57"/>
+      <c r="V8" s="57"/>
     </row>
     <row r="9" spans="1:45" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
@@ -2270,12 +2300,14 @@
       <c r="AB10" s="6"/>
       <c r="AL10" s="6"/>
     </row>
-    <row r="11" spans="1:45" ht="132" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" ht="168" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="78"/>
-      <c r="C11" s="77" t="s">
+      <c r="B11" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" s="54" t="s">
         <v>121</v>
       </c>
       <c r="D11" s="26" t="s">
@@ -2285,7 +2317,7 @@
         <v>120</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="G11" s="26" t="s">
         <v>122</v>
@@ -2316,7 +2348,9 @@
       <c r="A12" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="21"/>
+      <c r="B12" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="C12" s="21"/>
       <c r="D12" s="21" t="s">
         <v>123</v>
@@ -2352,7 +2386,9 @@
       <c r="A13" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="21"/>
+      <c r="B13" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21" t="s">
         <v>125</v>
@@ -2382,13 +2418,15 @@
       <c r="AR13" s="7"/>
       <c r="AS13" s="7"/>
     </row>
-    <row r="14" spans="1:45" ht="132" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" ht="156" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="21"/>
+      <c r="B14" s="21" t="s">
+        <v>133</v>
+      </c>
       <c r="C14" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>126</v>
@@ -2397,10 +2435,10 @@
         <v>124</v>
       </c>
       <c r="F14" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="G14" s="26" t="s">
         <v>127</v>
-      </c>
-      <c r="G14" s="26" t="s">
-        <v>128</v>
       </c>
       <c r="H14" s="26"/>
       <c r="I14" s="15"/>
@@ -2431,16 +2469,16 @@
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E15" s="26" t="s">
         <v>124</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H15" s="26"/>
       <c r="I15" s="15"/>
@@ -2464,16 +2502,26 @@
       <c r="AR15" s="7"/>
       <c r="AS15" s="7"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:45" ht="144" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
         <v>44</v>
       </c>
       <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
+      <c r="C16" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>135</v>
+      </c>
       <c r="H16" s="26"/>
       <c r="I16" s="15"/>
       <c r="J16" s="28"/>
@@ -2496,16 +2544,26 @@
       <c r="AR16" s="7"/>
       <c r="AS16" s="7"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:45" ht="144" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>45</v>
       </c>
       <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
+      <c r="C17" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>138</v>
+      </c>
       <c r="H17" s="26"/>
       <c r="I17" s="15"/>
       <c r="J17" s="28"/>
@@ -4530,98 +4588,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="70"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="68"/>
     </row>
     <row r="2" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="73" t="s">
+      <c r="B2" s="64"/>
+      <c r="C2" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="75"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="73" t="s">
+      <c r="D2" s="65"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="75"/>
-      <c r="H2" s="74"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="64"/>
       <c r="I2" s="51"/>
       <c r="J2" s="51"/>
       <c r="K2" s="52"/>
       <c r="L2" s="46"/>
     </row>
     <row r="3" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="70"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="68"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="76">
+      <c r="B4" s="76"/>
+      <c r="C4" s="53">
         <v>1</v>
       </c>
-      <c r="D4" s="61" t="s">
+      <c r="D4" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="63"/>
-      <c r="F4" s="76">
+      <c r="E4" s="72"/>
+      <c r="F4" s="53">
         <v>3</v>
       </c>
-      <c r="G4" s="61" t="s">
+      <c r="G4" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="H4" s="63"/>
+      <c r="H4" s="72"/>
       <c r="I4" s="45"/>
       <c r="J4" s="45"/>
       <c r="K4" s="45"/>
       <c r="L4" s="46"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="66"/>
-      <c r="B5" s="67"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="78"/>
       <c r="C5" s="47">
         <v>2</v>
       </c>
-      <c r="D5" s="60" t="s">
+      <c r="D5" s="73" t="s">
         <v>93</v>
       </c>
-      <c r="E5" s="72"/>
+      <c r="E5" s="70"/>
       <c r="F5" s="47">
         <v>4</v>
       </c>
-      <c r="G5" s="60" t="s">
+      <c r="G5" s="73" t="s">
         <v>95</v>
       </c>
-      <c r="H5" s="72"/>
+      <c r="H5" s="70"/>
       <c r="I5" s="45"/>
       <c r="J5" s="45"/>
       <c r="K5" s="45"/>
@@ -4631,35 +4689,35 @@
       <c r="A6" s="47"/>
       <c r="B6" s="46"/>
       <c r="C6" s="47"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="72"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="70"/>
       <c r="F6" s="47"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="72"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="70"/>
       <c r="I6" s="45"/>
       <c r="J6" s="45"/>
       <c r="K6" s="45"/>
       <c r="L6" s="46"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="72"/>
+      <c r="B7" s="70"/>
       <c r="C7" s="47">
         <v>5</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="D7" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="E7" s="72"/>
+      <c r="E7" s="70"/>
       <c r="F7" s="47">
         <v>6</v>
       </c>
-      <c r="G7" s="60" t="s">
+      <c r="G7" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="H7" s="72"/>
+      <c r="H7" s="70"/>
       <c r="I7" s="45"/>
       <c r="J7" s="45"/>
       <c r="K7" s="45"/>
@@ -4669,55 +4727,55 @@
       <c r="A8" s="47"/>
       <c r="B8" s="46"/>
       <c r="C8" s="47"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="72"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="47"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="72"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="70"/>
       <c r="I8" s="45"/>
       <c r="J8" s="45"/>
       <c r="K8" s="45"/>
       <c r="L8" s="46"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="67"/>
+      <c r="B9" s="78"/>
       <c r="C9" s="47">
         <v>6</v>
       </c>
-      <c r="D9" s="60" t="s">
+      <c r="D9" s="73" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="72"/>
+      <c r="E9" s="70"/>
       <c r="F9" s="47">
         <v>8</v>
       </c>
-      <c r="G9" s="60" t="s">
+      <c r="G9" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="H9" s="72"/>
+      <c r="H9" s="70"/>
       <c r="I9" s="45"/>
       <c r="J9" s="45"/>
       <c r="K9" s="45"/>
       <c r="L9" s="46"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="66"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="77"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="47">
         <v>7</v>
       </c>
-      <c r="D10" s="60" t="s">
+      <c r="D10" s="73" t="s">
         <v>101</v>
       </c>
-      <c r="E10" s="72"/>
+      <c r="E10" s="70"/>
       <c r="F10" s="47"/>
-      <c r="G10" s="60" t="s">
+      <c r="G10" s="73" t="s">
         <v>118</v>
       </c>
-      <c r="H10" s="72"/>
+      <c r="H10" s="70"/>
       <c r="I10" s="45"/>
       <c r="J10" s="45"/>
       <c r="K10" s="45"/>
@@ -4727,57 +4785,57 @@
       <c r="A11" s="47"/>
       <c r="B11" s="46"/>
       <c r="C11" s="47"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="72"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="70"/>
       <c r="F11" s="47"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="72"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="70"/>
       <c r="I11" s="45"/>
       <c r="J11" s="45"/>
       <c r="K11" s="45"/>
       <c r="L11" s="46"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="66" t="s">
+      <c r="A12" s="77" t="s">
         <v>103</v>
       </c>
-      <c r="B12" s="67"/>
+      <c r="B12" s="78"/>
       <c r="C12" s="47">
         <v>9</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="E12" s="72"/>
+      <c r="E12" s="70"/>
       <c r="F12" s="47">
         <v>11</v>
       </c>
-      <c r="G12" s="60" t="s">
+      <c r="G12" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="H12" s="72"/>
+      <c r="H12" s="70"/>
       <c r="I12" s="45"/>
       <c r="J12" s="45"/>
       <c r="K12" s="45"/>
       <c r="L12" s="46"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="66"/>
-      <c r="B13" s="67"/>
+      <c r="A13" s="77"/>
+      <c r="B13" s="78"/>
       <c r="C13" s="47">
         <v>10</v>
       </c>
-      <c r="D13" s="60" t="s">
+      <c r="D13" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="E13" s="72"/>
+      <c r="E13" s="70"/>
       <c r="F13" s="47">
         <v>12</v>
       </c>
-      <c r="G13" s="60" t="s">
+      <c r="G13" s="73" t="s">
         <v>107</v>
       </c>
-      <c r="H13" s="72"/>
+      <c r="H13" s="70"/>
       <c r="I13" s="45"/>
       <c r="J13" s="45"/>
       <c r="K13" s="45"/>
@@ -4787,15 +4845,15 @@
       <c r="A14" s="47"/>
       <c r="B14" s="46"/>
       <c r="C14" s="47"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="72"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="70"/>
       <c r="F14" s="47">
         <v>13</v>
       </c>
-      <c r="G14" s="60" t="s">
+      <c r="G14" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="H14" s="72"/>
+      <c r="H14" s="70"/>
       <c r="I14" s="45"/>
       <c r="J14" s="45"/>
       <c r="K14" s="45"/>
@@ -4805,50 +4863,50 @@
       <c r="A15" s="47"/>
       <c r="B15" s="46"/>
       <c r="C15" s="47"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="72"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="70"/>
       <c r="J15" s="45"/>
       <c r="K15" s="45"/>
       <c r="L15" s="46"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="67"/>
+      <c r="B16" s="78"/>
       <c r="C16" s="47">
         <v>14</v>
       </c>
-      <c r="D16" s="60" t="s">
+      <c r="D16" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="E16" s="72"/>
+      <c r="E16" s="70"/>
       <c r="F16" s="47">
         <v>16</v>
       </c>
-      <c r="G16" s="60" t="s">
+      <c r="G16" s="73" t="s">
         <v>112</v>
       </c>
-      <c r="H16" s="72"/>
+      <c r="H16" s="70"/>
       <c r="L16" s="45"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="66"/>
-      <c r="B17" s="67"/>
+      <c r="A17" s="77"/>
+      <c r="B17" s="78"/>
       <c r="C17" s="47">
         <v>15</v>
       </c>
-      <c r="D17" s="60" t="s">
+      <c r="D17" s="73" t="s">
         <v>111</v>
       </c>
-      <c r="E17" s="72"/>
+      <c r="E17" s="70"/>
       <c r="F17" s="47">
         <v>17</v>
       </c>
-      <c r="G17" s="60" t="s">
+      <c r="G17" s="73" t="s">
         <v>113</v>
       </c>
-      <c r="H17" s="72"/>
+      <c r="H17" s="70"/>
       <c r="I17" s="45"/>
       <c r="L17" s="45"/>
     </row>
@@ -4881,40 +4939,40 @@
       <c r="L19" s="46"/>
     </row>
     <row r="20" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="68" t="s">
+      <c r="A20" s="66" t="s">
         <v>114</v>
       </c>
-      <c r="B20" s="69"/>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="69"/>
-      <c r="I20" s="69"/>
-      <c r="J20" s="69"/>
-      <c r="K20" s="69"/>
-      <c r="L20" s="70"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="68"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="62" t="s">
+      <c r="A21" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="76">
+      <c r="B21" s="72"/>
+      <c r="C21" s="53">
         <v>18</v>
       </c>
-      <c r="D21" s="61" t="s">
+      <c r="D21" s="71" t="s">
         <v>116</v>
       </c>
-      <c r="E21" s="63"/>
-      <c r="F21" s="76">
+      <c r="E21" s="72"/>
+      <c r="F21" s="53">
         <v>19</v>
       </c>
-      <c r="G21" s="61" t="s">
+      <c r="G21" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="H21" s="63"/>
+      <c r="H21" s="72"/>
       <c r="I21" s="51"/>
       <c r="J21" s="51"/>
       <c r="K21" s="51"/>
@@ -5488,11 +5546,26 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A4:B5"/>
+    <mergeCell ref="A9:B10"/>
+    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="A16:B17"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
     <mergeCell ref="A20:L20"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="G4:H4"/>
@@ -5509,26 +5582,11 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A4:B5"/>
-    <mergeCell ref="A9:B10"/>
-    <mergeCell ref="A12:B13"/>
-    <mergeCell ref="A16:B17"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5794,6 +5852,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9EE5A02A2A6DC45B45E782DFEFDA45E" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7657f0a98c495c38e0a3edb0de0bfed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c79c8594d4fa4c9fd200c91a62336472" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -5919,24 +5994,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5952,22 +6028,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
cambio de clases y fotos
añadi clases de equivalencia y fotos ilustrativas
</commit_message>
<xml_diff>
--- a/ISW_Grupo6_4k2/Practicos/TP12/Resolucion_12_TestionMetodosCajaNegra.xlsx
+++ b/ISW_Grupo6_4k2/Practicos/TP12/Resolucion_12_TestionMetodosCajaNegra.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr hidePivotFieldList="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gaston\Documents\GitHub\ISW_Grupo6_4K2\ISW_Grupo6_4k2\Practicos\TP12\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9664657A-019A-4A60-8893-5FEF27643892}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="679" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos_Prueba" sheetId="27" r:id="rId1"/>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="235">
   <si>
     <t>TC_001</t>
   </si>
@@ -506,9 +512,6 @@
     <t>Realizar pedido "Lo que sea", seleccionando modo de pago "Tarjeta visa" y completando el campo "Nombre y Apellido" con números</t>
   </si>
   <si>
-    <t>1- Se selecciona opcion "Realizar nuevo pedido"   2-  No deja vacio el campo producto solicitado      3- No se adjunta foto                                                   4- Se ingresa direccion de local "Mariano fragueiro 1857, B° Alta cordoba"  y se selecciona ciudad "Cordoba"                                                                   5-Se ingresa la direccion de entrega "A. Sanchez ariño 2505"                                                                  6-Se ingresa forma de pago "TARJETA", se ingresa numero "4555000000000000", fecha de vencimiento "12/21" , se ingresa "Nombre y Apellido" 39393                7- Se ingresa recibirlo "LO ANTES POSIBLE"               8- Se confirma pedido.</t>
-  </si>
-  <si>
     <t>Se visualiza mensaje de error "Debe ingresar un nombre y apellido válidos"</t>
   </si>
   <si>
@@ -705,12 +708,39 @@
   </si>
   <si>
     <t>Dirrecion ingresada invalida</t>
+  </si>
+  <si>
+    <t>6,9,1,15,20,</t>
+  </si>
+  <si>
+    <t>6,9,1,2,15,20</t>
+  </si>
+  <si>
+    <t>6,9,5,13,20,</t>
+  </si>
+  <si>
+    <t>6,9,1,2,13,20,28</t>
+  </si>
+  <si>
+    <t>6,9,1,2,13,20</t>
+  </si>
+  <si>
+    <t>6,9,1,2,18,20,28</t>
+  </si>
+  <si>
+    <t>6,1,2,13,20</t>
+  </si>
+  <si>
+    <t>Foto ilustrativa</t>
+  </si>
+  <si>
+    <t>1- Se selecciona opcion "Realizar nuevo pedido"   2-  No deja vacio el campo producto solicitado      3- No se adjunta foto                                                   4- Se ingresa direccion de local "Mariano fragueiro 1857, B° Alta cordoba"  y se selecciona ciudad "Cordoba"                                                                   5-Se ingresa la direccion de entrega "A. Sanchez ariño 2505"                                                                  6-Se ingresa forma de pago "TARJETA", se ingresa numero "4555888888888", fecha de vencimiento "12/21" , se ingresa "Nombre y Apellido" 39393                7- Se ingresa recibirlo "LO ANTES POSIBLE"               8- Se confirma pedido.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -819,7 +849,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -877,6 +907,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1208,7 +1244,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -1372,40 +1408,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1417,29 +1447,55 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="DataPilot Category" xfId="1"/>
-    <cellStyle name="DataPilot Corner" xfId="2"/>
-    <cellStyle name="DataPilot Field" xfId="3"/>
-    <cellStyle name="DataPilot Result" xfId="4"/>
-    <cellStyle name="DataPilot Title" xfId="5"/>
-    <cellStyle name="DataPilot Value" xfId="6"/>
+    <cellStyle name="DataPilot Category" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="DataPilot Corner" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="DataPilot Field" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="DataPilot Result" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="DataPilot Title" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="DataPilot Value" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Neutral" xfId="7" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="8"/>
+    <cellStyle name="Normal 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Total" xfId="9" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="47">
@@ -1869,6 +1925,211 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2286000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>4064242</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D374EE70-3D2D-4DE2-8335-CD5FDA442A1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19069051" y="10058400"/>
+          <a:ext cx="2190749" cy="3892792"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>85102</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>70261</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2161309</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>3750300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF25A1FC-E8DC-44F8-BD08-C30B2C89AF3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19107393" y="24717497"/>
+          <a:ext cx="2076207" cy="3680039"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>221673</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>137009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2326697</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>3879273</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EB06E57-B615-426B-ADEC-B34E89C866BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19243964" y="19450245"/>
+          <a:ext cx="2105024" cy="3742264"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>221674</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>110836</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2325900</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>3837709</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagen 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8B28448-7166-405E-A857-010D6BCA7819}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19243965" y="32558181"/>
+          <a:ext cx="2104226" cy="3726873"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2216,44 +2477,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AS73"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="2" customWidth="1"/>
     <col min="2" max="3" width="10" style="2" customWidth="1"/>
-    <col min="4" max="4" width="43.140625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="38.140625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="43.109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="35.88671875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="38.109375" style="11" customWidth="1"/>
     <col min="7" max="7" width="52" style="12" customWidth="1"/>
     <col min="8" max="8" width="22" style="12" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" style="8" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" style="24" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="22" style="12" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="19.5703125" style="8" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="24" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="19.5546875" style="8" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" style="24" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="34.77734375" style="94" customWidth="1"/>
+    <col min="14" max="14" width="9.88671875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="19.5546875" style="8" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" style="24" customWidth="1"/>
+    <col min="17" max="17" width="12.44140625" style="2" customWidth="1"/>
     <col min="18" max="18" width="22" style="12" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" style="2" customWidth="1"/>
-    <col min="20" max="20" width="19.5703125" style="8" customWidth="1"/>
-    <col min="21" max="21" width="13.7109375" style="24" customWidth="1"/>
-    <col min="22" max="22" width="12.42578125" style="2" customWidth="1"/>
-    <col min="23" max="16384" width="11.42578125" style="2"/>
+    <col min="19" max="19" width="9.88671875" style="2" customWidth="1"/>
+    <col min="20" max="20" width="19.5546875" style="8" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" style="24" customWidth="1"/>
+    <col min="22" max="22" width="12.44140625" style="2" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" s="30"/>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -2266,7 +2527,7 @@
       <c r="J1" s="31"/>
       <c r="K1" s="31"/>
       <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
+      <c r="M1" s="91"/>
       <c r="N1" s="31"/>
       <c r="O1" s="31"/>
       <c r="P1" s="31"/>
@@ -2286,7 +2547,7 @@
       <c r="AD1" s="4"/>
       <c r="AE1" s="4"/>
     </row>
-    <row r="2" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="64" t="s">
         <v>63</v>
       </c>
@@ -2301,7 +2562,7 @@
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
       <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
+      <c r="M2" s="92"/>
       <c r="N2" s="32"/>
       <c r="O2" s="32"/>
       <c r="P2" s="32"/>
@@ -2321,7 +2582,7 @@
       <c r="AD2" s="4"/>
       <c r="AE2" s="4"/>
     </row>
-    <row r="3" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="64"/>
       <c r="B3" s="64"/>
       <c r="C3" s="64"/>
@@ -2334,7 +2595,7 @@
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
       <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
+      <c r="M3" s="92"/>
       <c r="N3" s="32"/>
       <c r="O3" s="32"/>
       <c r="P3" s="32"/>
@@ -2354,7 +2615,7 @@
       <c r="AD3" s="4"/>
       <c r="AE3" s="4"/>
     </row>
-    <row r="4" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="64"/>
       <c r="B4" s="64"/>
       <c r="C4" s="64"/>
@@ -2367,7 +2628,7 @@
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
       <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
+      <c r="M4" s="92"/>
       <c r="N4" s="32"/>
       <c r="O4" s="32"/>
       <c r="P4" s="32"/>
@@ -2387,7 +2648,7 @@
       <c r="AD4" s="4"/>
       <c r="AE4" s="4"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" s="66" t="s">
         <v>64</v>
       </c>
@@ -2402,7 +2663,7 @@
       <c r="J5" s="33"/>
       <c r="K5" s="33"/>
       <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
+      <c r="M5" s="93"/>
       <c r="N5" s="33"/>
       <c r="O5" s="33"/>
       <c r="P5" s="33"/>
@@ -2421,14 +2682,14 @@
       <c r="AC5" s="4"/>
       <c r="AD5" s="4"/>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="34"/>
       <c r="K6" s="35"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="M6" s="34"/>
       <c r="N6" s="4"/>
       <c r="O6" s="34"/>
       <c r="P6" s="35"/>
@@ -2447,8 +2708,8 @@
       <c r="AC6" s="4"/>
       <c r="AD6" s="4"/>
     </row>
-    <row r="7" spans="1:45" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:45" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:45" s="1" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="67"/>
       <c r="B8" s="67"/>
       <c r="C8" s="67"/>
@@ -2478,7 +2739,7 @@
       <c r="U8" s="65"/>
       <c r="V8" s="65"/>
     </row>
-    <row r="9" spans="1:45" ht="24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:45" ht="24" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>65</v>
       </c>
@@ -2515,8 +2776,8 @@
       <c r="L9" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="M9" s="14" t="s">
-        <v>71</v>
+      <c r="M9" s="95" t="s">
+        <v>233</v>
       </c>
       <c r="N9" s="14" t="s">
         <v>72</v>
@@ -2548,7 +2809,7 @@
       <c r="AB9" s="3"/>
       <c r="AL9" s="3"/>
     </row>
-    <row r="10" spans="1:45" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:45" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
@@ -2561,7 +2822,7 @@
       <c r="J10" s="18"/>
       <c r="K10" s="23"/>
       <c r="L10" s="36"/>
-      <c r="M10" s="38"/>
+      <c r="M10" s="96"/>
       <c r="N10" s="18"/>
       <c r="O10" s="18"/>
       <c r="P10" s="23"/>
@@ -2574,7 +2835,7 @@
       <c r="AB10" s="6"/>
       <c r="AL10" s="6"/>
     </row>
-    <row r="11" spans="1:45" ht="168" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:45" ht="144" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>0</v>
       </c>
@@ -2609,7 +2870,7 @@
       <c r="L11" s="58">
         <v>43753</v>
       </c>
-      <c r="M11" s="15"/>
+      <c r="M11" s="97"/>
       <c r="N11" s="28"/>
       <c r="O11" s="29"/>
       <c r="P11" s="16"/>
@@ -2626,7 +2887,7 @@
       <c r="AR11" s="7"/>
       <c r="AS11" s="7"/>
     </row>
-    <row r="12" spans="1:45" ht="216" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:45" ht="180" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>40</v>
       </c>
@@ -2634,7 +2895,7 @@
         <v>126</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>119</v>
@@ -2659,7 +2920,7 @@
       <c r="L12" s="37">
         <v>43753</v>
       </c>
-      <c r="M12" s="39"/>
+      <c r="M12" s="98"/>
       <c r="N12" s="15"/>
       <c r="O12" s="28"/>
       <c r="P12" s="29"/>
@@ -2676,7 +2937,7 @@
       <c r="AR12" s="7"/>
       <c r="AS12" s="7"/>
     </row>
-    <row r="13" spans="1:45" ht="167.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" ht="167.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>41</v>
       </c>
@@ -2684,7 +2945,7 @@
         <v>126</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>121</v>
@@ -2707,7 +2968,7 @@
       <c r="J13" s="28"/>
       <c r="K13" s="29"/>
       <c r="L13" s="37"/>
-      <c r="M13" s="39"/>
+      <c r="M13" s="98"/>
       <c r="N13" s="15"/>
       <c r="O13" s="28"/>
       <c r="P13" s="29"/>
@@ -2724,7 +2985,7 @@
       <c r="AR13" s="7"/>
       <c r="AS13" s="7"/>
     </row>
-    <row r="14" spans="1:45" ht="168" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" ht="144" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>42</v>
       </c>
@@ -2757,7 +3018,7 @@
       <c r="L14" s="37">
         <v>43753</v>
       </c>
-      <c r="M14" s="39"/>
+      <c r="M14" s="98"/>
       <c r="N14" s="15"/>
       <c r="O14" s="28"/>
       <c r="P14" s="29"/>
@@ -2774,7 +3035,7 @@
       <c r="AR14" s="7"/>
       <c r="AS14" s="7"/>
     </row>
-    <row r="15" spans="1:45" ht="120" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:45" ht="328.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>43</v>
       </c>
@@ -2782,7 +3043,7 @@
         <v>127</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>124</v>
@@ -2811,7 +3072,7 @@
       <c r="L15" s="37">
         <v>43753</v>
       </c>
-      <c r="M15" s="39"/>
+      <c r="M15" s="98"/>
       <c r="N15" s="15"/>
       <c r="O15" s="28"/>
       <c r="P15" s="29"/>
@@ -2828,7 +3089,7 @@
       <c r="AR15" s="7"/>
       <c r="AS15" s="7"/>
     </row>
-    <row r="16" spans="1:45" ht="144" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:45" ht="132" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>44</v>
       </c>
@@ -2863,7 +3124,7 @@
       <c r="L16" s="37">
         <v>43753</v>
       </c>
-      <c r="M16" s="39"/>
+      <c r="M16" s="98"/>
       <c r="N16" s="15"/>
       <c r="O16" s="28"/>
       <c r="P16" s="29"/>
@@ -2880,7 +3141,7 @@
       <c r="AR16" s="7"/>
       <c r="AS16" s="7"/>
     </row>
-    <row r="17" spans="1:45" ht="144" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:45" ht="132" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>45</v>
       </c>
@@ -2915,7 +3176,7 @@
       <c r="L17" s="37">
         <v>43753</v>
       </c>
-      <c r="M17" s="39"/>
+      <c r="M17" s="98"/>
       <c r="N17" s="15"/>
       <c r="O17" s="28"/>
       <c r="P17" s="29"/>
@@ -2932,7 +3193,7 @@
       <c r="AR17" s="7"/>
       <c r="AS17" s="7"/>
     </row>
-    <row r="18" spans="1:45" ht="156" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:45" ht="144" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>46</v>
       </c>
@@ -2967,7 +3228,7 @@
       <c r="L18" s="37">
         <v>43753</v>
       </c>
-      <c r="M18" s="39"/>
+      <c r="M18" s="98"/>
       <c r="N18" s="15"/>
       <c r="O18" s="28"/>
       <c r="P18" s="29"/>
@@ -2984,14 +3245,16 @@
       <c r="AR18" s="7"/>
       <c r="AS18" s="7"/>
     </row>
-    <row r="19" spans="1:45" ht="168" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:45" ht="316.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="C19" s="21"/>
+      <c r="C19" s="90" t="s">
+        <v>226</v>
+      </c>
       <c r="D19" s="21" t="s">
         <v>159</v>
       </c>
@@ -2999,10 +3262,10 @@
         <v>120</v>
       </c>
       <c r="F19" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="G19" s="26" t="s">
         <v>160</v>
-      </c>
-      <c r="G19" s="26" t="s">
-        <v>161</v>
       </c>
       <c r="H19" s="26" t="s">
         <v>135</v>
@@ -3017,7 +3280,7 @@
       <c r="L19" s="37">
         <v>43753</v>
       </c>
-      <c r="M19" s="39"/>
+      <c r="M19" s="98"/>
       <c r="N19" s="15"/>
       <c r="O19" s="28"/>
       <c r="P19" s="29"/>
@@ -3034,25 +3297,27 @@
       <c r="AR19" s="7"/>
       <c r="AS19" s="7"/>
     </row>
-    <row r="20" spans="1:45" ht="168" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:45" ht="144" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>48</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="21"/>
+      <c r="C20" s="90" t="s">
+        <v>227</v>
+      </c>
       <c r="D20" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E20" s="26" t="s">
         <v>120</v>
       </c>
       <c r="F20" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="G20" s="26" t="s">
         <v>163</v>
-      </c>
-      <c r="G20" s="26" t="s">
-        <v>164</v>
       </c>
       <c r="H20" s="26" t="s">
         <v>135</v>
@@ -3067,7 +3332,7 @@
       <c r="L20" s="37">
         <v>43753</v>
       </c>
-      <c r="M20" s="39"/>
+      <c r="M20" s="98"/>
       <c r="N20" s="15"/>
       <c r="O20" s="28"/>
       <c r="P20" s="29"/>
@@ -3084,25 +3349,27 @@
       <c r="AR20" s="7"/>
       <c r="AS20" s="7"/>
     </row>
-    <row r="21" spans="1:45" ht="132" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:45" ht="132" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>49</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="C21" s="21"/>
+      <c r="C21" s="21" t="s">
+        <v>228</v>
+      </c>
       <c r="D21" s="21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E21" s="26" t="s">
         <v>120</v>
       </c>
       <c r="F21" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="G21" s="26" t="s">
         <v>166</v>
-      </c>
-      <c r="G21" s="26" t="s">
-        <v>167</v>
       </c>
       <c r="H21" s="26" t="s">
         <v>135</v>
@@ -3117,7 +3384,7 @@
       <c r="L21" s="37">
         <v>43753</v>
       </c>
-      <c r="M21" s="39"/>
+      <c r="M21" s="98"/>
       <c r="N21" s="15"/>
       <c r="O21" s="28"/>
       <c r="P21" s="29"/>
@@ -3134,28 +3401,30 @@
       <c r="AR21" s="7"/>
       <c r="AS21" s="7"/>
     </row>
-    <row r="22" spans="1:45" ht="156" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:45" ht="297.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
         <v>50</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="C22" s="21"/>
+      <c r="C22" s="21" t="s">
+        <v>229</v>
+      </c>
       <c r="D22" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E22" s="26" t="s">
         <v>120</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G22" s="26" t="s">
         <v>135</v>
       </c>
       <c r="H22" s="26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I22" s="15" t="s">
         <v>147</v>
@@ -3167,7 +3436,7 @@
       <c r="L22" s="37">
         <v>43753</v>
       </c>
-      <c r="M22" s="39"/>
+      <c r="M22" s="98"/>
       <c r="N22" s="15"/>
       <c r="O22" s="28"/>
       <c r="P22" s="29"/>
@@ -3184,25 +3453,27 @@
       <c r="AR22" s="7"/>
       <c r="AS22" s="7"/>
     </row>
-    <row r="23" spans="1:45" ht="156" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:45" ht="144" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>51</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="C23" s="21"/>
+      <c r="C23" s="90" t="s">
+        <v>230</v>
+      </c>
       <c r="D23" s="21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E23" s="26" t="s">
         <v>120</v>
       </c>
       <c r="F23" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="G23" s="26" t="s">
         <v>173</v>
-      </c>
-      <c r="G23" s="26" t="s">
-        <v>174</v>
       </c>
       <c r="H23" s="26" t="s">
         <v>135</v>
@@ -3217,7 +3488,7 @@
       <c r="L23" s="37">
         <v>43753</v>
       </c>
-      <c r="M23" s="39"/>
+      <c r="M23" s="98"/>
       <c r="N23" s="15"/>
       <c r="O23" s="28"/>
       <c r="P23" s="29"/>
@@ -3234,25 +3505,27 @@
       <c r="AR23" s="7"/>
       <c r="AS23" s="7"/>
     </row>
-    <row r="24" spans="1:45" ht="156" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:45" ht="307.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
         <v>52</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="C24" s="21"/>
+      <c r="C24" s="21" t="s">
+        <v>231</v>
+      </c>
       <c r="D24" s="21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E24" s="26" t="s">
         <v>120</v>
       </c>
       <c r="F24" s="26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G24" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H24" s="26" t="s">
         <v>135</v>
@@ -3267,7 +3540,7 @@
       <c r="L24" s="37">
         <v>43753</v>
       </c>
-      <c r="M24" s="39"/>
+      <c r="M24" s="98"/>
       <c r="N24" s="15"/>
       <c r="O24" s="28"/>
       <c r="P24" s="29"/>
@@ -3284,7 +3557,7 @@
       <c r="AR24" s="7"/>
       <c r="AS24" s="7"/>
     </row>
-    <row r="25" spans="1:45" ht="168" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:45" ht="144" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>53</v>
       </c>
@@ -3292,22 +3565,22 @@
         <v>158</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E25" s="26" t="s">
         <v>120</v>
       </c>
       <c r="F25" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="G25" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="G25" s="26" t="s">
+      <c r="H25" s="26" t="s">
         <v>189</v>
-      </c>
-      <c r="H25" s="26" t="s">
-        <v>190</v>
       </c>
       <c r="I25" s="15" t="s">
         <v>147</v>
@@ -3319,7 +3592,7 @@
       <c r="L25" s="37">
         <v>43753</v>
       </c>
-      <c r="M25" s="39"/>
+      <c r="M25" s="98"/>
       <c r="N25" s="15"/>
       <c r="O25" s="28"/>
       <c r="P25" s="29"/>
@@ -3336,28 +3609,30 @@
       <c r="AR25" s="7"/>
       <c r="AS25" s="7"/>
     </row>
-    <row r="26" spans="1:45" ht="192" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:45" ht="132" x14ac:dyDescent="0.3">
       <c r="A26" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="C26" s="21"/>
+      <c r="C26" s="21" t="s">
+        <v>232</v>
+      </c>
       <c r="D26" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E26" s="26" t="s">
         <v>133</v>
       </c>
       <c r="F26" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G26" s="26" t="s">
         <v>135</v>
       </c>
       <c r="H26" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I26" s="15" t="s">
         <v>147</v>
@@ -3369,7 +3644,7 @@
       <c r="L26" s="37">
         <v>43753</v>
       </c>
-      <c r="M26" s="39"/>
+      <c r="M26" s="98"/>
       <c r="N26" s="15"/>
       <c r="O26" s="28"/>
       <c r="P26" s="29"/>
@@ -3386,7 +3661,7 @@
       <c r="AR26" s="7"/>
       <c r="AS26" s="7"/>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>55</v>
       </c>
@@ -3401,7 +3676,7 @@
       <c r="J27" s="28"/>
       <c r="K27" s="29"/>
       <c r="L27" s="37"/>
-      <c r="M27" s="39"/>
+      <c r="M27" s="98"/>
       <c r="N27" s="15"/>
       <c r="O27" s="28"/>
       <c r="P27" s="29"/>
@@ -3418,7 +3693,7 @@
       <c r="AR27" s="7"/>
       <c r="AS27" s="7"/>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A28" s="20" t="s">
         <v>56</v>
       </c>
@@ -3433,7 +3708,7 @@
       <c r="J28" s="28"/>
       <c r="K28" s="29"/>
       <c r="L28" s="37"/>
-      <c r="M28" s="39"/>
+      <c r="M28" s="98"/>
       <c r="N28" s="15"/>
       <c r="O28" s="28"/>
       <c r="P28" s="29"/>
@@ -3450,7 +3725,7 @@
       <c r="AR28" s="7"/>
       <c r="AS28" s="7"/>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
         <v>57</v>
       </c>
@@ -3465,7 +3740,7 @@
       <c r="J29" s="28"/>
       <c r="K29" s="29"/>
       <c r="L29" s="37"/>
-      <c r="M29" s="39"/>
+      <c r="M29" s="98"/>
       <c r="N29" s="15"/>
       <c r="O29" s="28"/>
       <c r="P29" s="29"/>
@@ -3482,7 +3757,7 @@
       <c r="AR29" s="7"/>
       <c r="AS29" s="7"/>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
         <v>58</v>
       </c>
@@ -3497,7 +3772,7 @@
       <c r="J30" s="28"/>
       <c r="K30" s="29"/>
       <c r="L30" s="37"/>
-      <c r="M30" s="39"/>
+      <c r="M30" s="98"/>
       <c r="N30" s="15"/>
       <c r="O30" s="28"/>
       <c r="P30" s="29"/>
@@ -3514,7 +3789,7 @@
       <c r="AR30" s="7"/>
       <c r="AS30" s="7"/>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
         <v>59</v>
       </c>
@@ -3529,7 +3804,7 @@
       <c r="J31" s="28"/>
       <c r="K31" s="29"/>
       <c r="L31" s="37"/>
-      <c r="M31" s="39"/>
+      <c r="M31" s="98"/>
       <c r="N31" s="15"/>
       <c r="O31" s="28"/>
       <c r="P31" s="29"/>
@@ -3546,7 +3821,7 @@
       <c r="AR31" s="7"/>
       <c r="AS31" s="7"/>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
         <v>60</v>
       </c>
@@ -3561,7 +3836,7 @@
       <c r="J32" s="28"/>
       <c r="K32" s="29"/>
       <c r="L32" s="37"/>
-      <c r="M32" s="39"/>
+      <c r="M32" s="98"/>
       <c r="N32" s="15"/>
       <c r="O32" s="28"/>
       <c r="P32" s="29"/>
@@ -3578,7 +3853,7 @@
       <c r="AR32" s="7"/>
       <c r="AS32" s="7"/>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>61</v>
       </c>
@@ -3593,7 +3868,7 @@
       <c r="J33" s="28"/>
       <c r="K33" s="29"/>
       <c r="L33" s="37"/>
-      <c r="M33" s="39"/>
+      <c r="M33" s="98"/>
       <c r="N33" s="15"/>
       <c r="O33" s="28"/>
       <c r="P33" s="29"/>
@@ -3610,7 +3885,7 @@
       <c r="AR33" s="7"/>
       <c r="AS33" s="7"/>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A34" s="20" t="s">
         <v>62</v>
       </c>
@@ -3625,7 +3900,7 @@
       <c r="J34" s="28"/>
       <c r="K34" s="29"/>
       <c r="L34" s="37"/>
-      <c r="M34" s="39"/>
+      <c r="M34" s="98"/>
       <c r="N34" s="15"/>
       <c r="O34" s="28"/>
       <c r="P34" s="29"/>
@@ -3642,7 +3917,7 @@
       <c r="AR34" s="7"/>
       <c r="AS34" s="7"/>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>1</v>
       </c>
@@ -3657,7 +3932,7 @@
       <c r="J35" s="28"/>
       <c r="K35" s="29"/>
       <c r="L35" s="37"/>
-      <c r="M35" s="39"/>
+      <c r="M35" s="98"/>
       <c r="N35" s="15"/>
       <c r="O35" s="28"/>
       <c r="P35" s="29"/>
@@ -3674,7 +3949,7 @@
       <c r="AR35" s="7"/>
       <c r="AS35" s="7"/>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A36" s="20" t="s">
         <v>2</v>
       </c>
@@ -3689,7 +3964,7 @@
       <c r="J36" s="28"/>
       <c r="K36" s="29"/>
       <c r="L36" s="37"/>
-      <c r="M36" s="39"/>
+      <c r="M36" s="98"/>
       <c r="N36" s="15"/>
       <c r="O36" s="28"/>
       <c r="P36" s="29"/>
@@ -3706,7 +3981,7 @@
       <c r="AR36" s="7"/>
       <c r="AS36" s="7"/>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>3</v>
       </c>
@@ -3721,7 +3996,7 @@
       <c r="J37" s="28"/>
       <c r="K37" s="29"/>
       <c r="L37" s="37"/>
-      <c r="M37" s="39"/>
+      <c r="M37" s="98"/>
       <c r="N37" s="15"/>
       <c r="O37" s="28"/>
       <c r="P37" s="29"/>
@@ -3738,7 +4013,7 @@
       <c r="AR37" s="7"/>
       <c r="AS37" s="7"/>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
         <v>4</v>
       </c>
@@ -3753,7 +4028,7 @@
       <c r="J38" s="28"/>
       <c r="K38" s="29"/>
       <c r="L38" s="37"/>
-      <c r="M38" s="39"/>
+      <c r="M38" s="98"/>
       <c r="N38" s="15"/>
       <c r="O38" s="28"/>
       <c r="P38" s="29"/>
@@ -3770,7 +4045,7 @@
       <c r="AR38" s="7"/>
       <c r="AS38" s="7"/>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
         <v>5</v>
       </c>
@@ -3785,7 +4060,7 @@
       <c r="J39" s="28"/>
       <c r="K39" s="29"/>
       <c r="L39" s="37"/>
-      <c r="M39" s="39"/>
+      <c r="M39" s="98"/>
       <c r="N39" s="15"/>
       <c r="O39" s="28"/>
       <c r="P39" s="29"/>
@@ -3802,7 +4077,7 @@
       <c r="AR39" s="7"/>
       <c r="AS39" s="7"/>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A40" s="20" t="s">
         <v>6</v>
       </c>
@@ -3817,7 +4092,7 @@
       <c r="J40" s="28"/>
       <c r="K40" s="29"/>
       <c r="L40" s="37"/>
-      <c r="M40" s="39"/>
+      <c r="M40" s="98"/>
       <c r="N40" s="15"/>
       <c r="O40" s="28"/>
       <c r="P40" s="29"/>
@@ -3834,7 +4109,7 @@
       <c r="AR40" s="7"/>
       <c r="AS40" s="7"/>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
         <v>7</v>
       </c>
@@ -3849,7 +4124,7 @@
       <c r="J41" s="28"/>
       <c r="K41" s="29"/>
       <c r="L41" s="37"/>
-      <c r="M41" s="39"/>
+      <c r="M41" s="98"/>
       <c r="N41" s="15"/>
       <c r="O41" s="28"/>
       <c r="P41" s="29"/>
@@ -3866,7 +4141,7 @@
       <c r="AR41" s="7"/>
       <c r="AS41" s="7"/>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A42" s="20" t="s">
         <v>8</v>
       </c>
@@ -3881,7 +4156,7 @@
       <c r="J42" s="28"/>
       <c r="K42" s="29"/>
       <c r="L42" s="37"/>
-      <c r="M42" s="39"/>
+      <c r="M42" s="98"/>
       <c r="N42" s="15"/>
       <c r="O42" s="28"/>
       <c r="P42" s="29"/>
@@ -3898,7 +4173,7 @@
       <c r="AR42" s="7"/>
       <c r="AS42" s="7"/>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
         <v>9</v>
       </c>
@@ -3913,7 +4188,7 @@
       <c r="J43" s="28"/>
       <c r="K43" s="29"/>
       <c r="L43" s="37"/>
-      <c r="M43" s="39"/>
+      <c r="M43" s="98"/>
       <c r="N43" s="15"/>
       <c r="O43" s="28"/>
       <c r="P43" s="29"/>
@@ -3930,7 +4205,7 @@
       <c r="AR43" s="7"/>
       <c r="AS43" s="7"/>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A44" s="20" t="s">
         <v>10</v>
       </c>
@@ -3945,7 +4220,7 @@
       <c r="J44" s="28"/>
       <c r="K44" s="29"/>
       <c r="L44" s="37"/>
-      <c r="M44" s="39"/>
+      <c r="M44" s="98"/>
       <c r="N44" s="15"/>
       <c r="O44" s="28"/>
       <c r="P44" s="29"/>
@@ -3962,7 +4237,7 @@
       <c r="AR44" s="7"/>
       <c r="AS44" s="7"/>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A45" s="20" t="s">
         <v>11</v>
       </c>
@@ -3977,7 +4252,7 @@
       <c r="J45" s="28"/>
       <c r="K45" s="29"/>
       <c r="L45" s="37"/>
-      <c r="M45" s="39"/>
+      <c r="M45" s="98"/>
       <c r="N45" s="15"/>
       <c r="O45" s="28"/>
       <c r="P45" s="29"/>
@@ -3994,7 +4269,7 @@
       <c r="AR45" s="7"/>
       <c r="AS45" s="7"/>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A46" s="20" t="s">
         <v>12</v>
       </c>
@@ -4009,7 +4284,7 @@
       <c r="J46" s="28"/>
       <c r="K46" s="29"/>
       <c r="L46" s="37"/>
-      <c r="M46" s="39"/>
+      <c r="M46" s="98"/>
       <c r="N46" s="15"/>
       <c r="O46" s="28"/>
       <c r="P46" s="29"/>
@@ -4026,7 +4301,7 @@
       <c r="AR46" s="7"/>
       <c r="AS46" s="7"/>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
         <v>13</v>
       </c>
@@ -4041,7 +4316,7 @@
       <c r="J47" s="28"/>
       <c r="K47" s="29"/>
       <c r="L47" s="37"/>
-      <c r="M47" s="39"/>
+      <c r="M47" s="98"/>
       <c r="N47" s="15"/>
       <c r="O47" s="28"/>
       <c r="P47" s="29"/>
@@ -4058,7 +4333,7 @@
       <c r="AR47" s="7"/>
       <c r="AS47" s="7"/>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A48" s="20" t="s">
         <v>14</v>
       </c>
@@ -4073,7 +4348,7 @@
       <c r="J48" s="28"/>
       <c r="K48" s="29"/>
       <c r="L48" s="37"/>
-      <c r="M48" s="39"/>
+      <c r="M48" s="98"/>
       <c r="N48" s="15"/>
       <c r="O48" s="28"/>
       <c r="P48" s="29"/>
@@ -4090,7 +4365,7 @@
       <c r="AR48" s="7"/>
       <c r="AS48" s="7"/>
     </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
         <v>15</v>
       </c>
@@ -4105,7 +4380,7 @@
       <c r="J49" s="28"/>
       <c r="K49" s="29"/>
       <c r="L49" s="37"/>
-      <c r="M49" s="39"/>
+      <c r="M49" s="98"/>
       <c r="N49" s="15"/>
       <c r="O49" s="28"/>
       <c r="P49" s="29"/>
@@ -4122,7 +4397,7 @@
       <c r="AR49" s="7"/>
       <c r="AS49" s="7"/>
     </row>
-    <row r="50" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A50" s="20" t="s">
         <v>16</v>
       </c>
@@ -4137,7 +4412,7 @@
       <c r="J50" s="28"/>
       <c r="K50" s="29"/>
       <c r="L50" s="37"/>
-      <c r="M50" s="39"/>
+      <c r="M50" s="98"/>
       <c r="N50" s="15"/>
       <c r="O50" s="28"/>
       <c r="P50" s="29"/>
@@ -4154,7 +4429,7 @@
       <c r="AR50" s="7"/>
       <c r="AS50" s="7"/>
     </row>
-    <row r="51" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="s">
         <v>17</v>
       </c>
@@ -4169,7 +4444,7 @@
       <c r="J51" s="28"/>
       <c r="K51" s="29"/>
       <c r="L51" s="37"/>
-      <c r="M51" s="39"/>
+      <c r="M51" s="98"/>
       <c r="N51" s="15"/>
       <c r="O51" s="28"/>
       <c r="P51" s="29"/>
@@ -4186,7 +4461,7 @@
       <c r="AR51" s="7"/>
       <c r="AS51" s="7"/>
     </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A52" s="20" t="s">
         <v>18</v>
       </c>
@@ -4201,7 +4476,7 @@
       <c r="J52" s="28"/>
       <c r="K52" s="29"/>
       <c r="L52" s="37"/>
-      <c r="M52" s="39"/>
+      <c r="M52" s="98"/>
       <c r="N52" s="15"/>
       <c r="O52" s="28"/>
       <c r="P52" s="29"/>
@@ -4218,7 +4493,7 @@
       <c r="AR52" s="7"/>
       <c r="AS52" s="7"/>
     </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A53" s="20" t="s">
         <v>19</v>
       </c>
@@ -4233,7 +4508,7 @@
       <c r="J53" s="28"/>
       <c r="K53" s="29"/>
       <c r="L53" s="37"/>
-      <c r="M53" s="39"/>
+      <c r="M53" s="98"/>
       <c r="N53" s="15"/>
       <c r="O53" s="28"/>
       <c r="P53" s="29"/>
@@ -4250,7 +4525,7 @@
       <c r="AR53" s="7"/>
       <c r="AS53" s="7"/>
     </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A54" s="20" t="s">
         <v>20</v>
       </c>
@@ -4265,7 +4540,7 @@
       <c r="J54" s="28"/>
       <c r="K54" s="29"/>
       <c r="L54" s="37"/>
-      <c r="M54" s="39"/>
+      <c r="M54" s="98"/>
       <c r="N54" s="15"/>
       <c r="O54" s="28"/>
       <c r="P54" s="29"/>
@@ -4282,7 +4557,7 @@
       <c r="AR54" s="7"/>
       <c r="AS54" s="7"/>
     </row>
-    <row r="55" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A55" s="20" t="s">
         <v>21</v>
       </c>
@@ -4297,7 +4572,7 @@
       <c r="J55" s="28"/>
       <c r="K55" s="29"/>
       <c r="L55" s="37"/>
-      <c r="M55" s="39"/>
+      <c r="M55" s="98"/>
       <c r="N55" s="15"/>
       <c r="O55" s="28"/>
       <c r="P55" s="29"/>
@@ -4314,7 +4589,7 @@
       <c r="AR55" s="7"/>
       <c r="AS55" s="7"/>
     </row>
-    <row r="56" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A56" s="20" t="s">
         <v>22</v>
       </c>
@@ -4329,7 +4604,7 @@
       <c r="J56" s="28"/>
       <c r="K56" s="29"/>
       <c r="L56" s="37"/>
-      <c r="M56" s="39"/>
+      <c r="M56" s="98"/>
       <c r="N56" s="15"/>
       <c r="O56" s="28"/>
       <c r="P56" s="29"/>
@@ -4346,7 +4621,7 @@
       <c r="AR56" s="7"/>
       <c r="AS56" s="7"/>
     </row>
-    <row r="57" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A57" s="20" t="s">
         <v>23</v>
       </c>
@@ -4361,7 +4636,7 @@
       <c r="J57" s="28"/>
       <c r="K57" s="29"/>
       <c r="L57" s="37"/>
-      <c r="M57" s="39"/>
+      <c r="M57" s="98"/>
       <c r="N57" s="15"/>
       <c r="O57" s="28"/>
       <c r="P57" s="29"/>
@@ -4378,7 +4653,7 @@
       <c r="AR57" s="7"/>
       <c r="AS57" s="7"/>
     </row>
-    <row r="58" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A58" s="20" t="s">
         <v>24</v>
       </c>
@@ -4393,7 +4668,7 @@
       <c r="J58" s="28"/>
       <c r="K58" s="29"/>
       <c r="L58" s="37"/>
-      <c r="M58" s="39"/>
+      <c r="M58" s="98"/>
       <c r="N58" s="15"/>
       <c r="O58" s="28"/>
       <c r="P58" s="29"/>
@@ -4410,7 +4685,7 @@
       <c r="AR58" s="7"/>
       <c r="AS58" s="7"/>
     </row>
-    <row r="59" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A59" s="20" t="s">
         <v>25</v>
       </c>
@@ -4425,7 +4700,7 @@
       <c r="J59" s="28"/>
       <c r="K59" s="29"/>
       <c r="L59" s="37"/>
-      <c r="M59" s="39"/>
+      <c r="M59" s="98"/>
       <c r="N59" s="15"/>
       <c r="O59" s="28"/>
       <c r="P59" s="29"/>
@@ -4442,7 +4717,7 @@
       <c r="AR59" s="7"/>
       <c r="AS59" s="7"/>
     </row>
-    <row r="60" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A60" s="20" t="s">
         <v>26</v>
       </c>
@@ -4457,7 +4732,7 @@
       <c r="J60" s="28"/>
       <c r="K60" s="29"/>
       <c r="L60" s="37"/>
-      <c r="M60" s="39"/>
+      <c r="M60" s="98"/>
       <c r="N60" s="15"/>
       <c r="O60" s="28"/>
       <c r="P60" s="29"/>
@@ -4474,7 +4749,7 @@
       <c r="AR60" s="7"/>
       <c r="AS60" s="7"/>
     </row>
-    <row r="61" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
         <v>27</v>
       </c>
@@ -4489,7 +4764,7 @@
       <c r="J61" s="28"/>
       <c r="K61" s="29"/>
       <c r="L61" s="37"/>
-      <c r="M61" s="39"/>
+      <c r="M61" s="98"/>
       <c r="N61" s="15"/>
       <c r="O61" s="28"/>
       <c r="P61" s="29"/>
@@ -4506,7 +4781,7 @@
       <c r="AR61" s="7"/>
       <c r="AS61" s="7"/>
     </row>
-    <row r="62" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A62" s="20" t="s">
         <v>28</v>
       </c>
@@ -4521,7 +4796,7 @@
       <c r="J62" s="28"/>
       <c r="K62" s="29"/>
       <c r="L62" s="37"/>
-      <c r="M62" s="39"/>
+      <c r="M62" s="98"/>
       <c r="N62" s="15"/>
       <c r="O62" s="28"/>
       <c r="P62" s="29"/>
@@ -4538,7 +4813,7 @@
       <c r="AR62" s="7"/>
       <c r="AS62" s="7"/>
     </row>
-    <row r="63" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A63" s="20" t="s">
         <v>29</v>
       </c>
@@ -4553,7 +4828,7 @@
       <c r="J63" s="28"/>
       <c r="K63" s="29"/>
       <c r="L63" s="37"/>
-      <c r="M63" s="39"/>
+      <c r="M63" s="98"/>
       <c r="N63" s="15"/>
       <c r="O63" s="28"/>
       <c r="P63" s="29"/>
@@ -4570,7 +4845,7 @@
       <c r="AR63" s="7"/>
       <c r="AS63" s="7"/>
     </row>
-    <row r="64" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
         <v>30</v>
       </c>
@@ -4585,7 +4860,7 @@
       <c r="J64" s="28"/>
       <c r="K64" s="29"/>
       <c r="L64" s="37"/>
-      <c r="M64" s="39"/>
+      <c r="M64" s="98"/>
       <c r="N64" s="15"/>
       <c r="O64" s="28"/>
       <c r="P64" s="29"/>
@@ -4602,7 +4877,7 @@
       <c r="AR64" s="7"/>
       <c r="AS64" s="7"/>
     </row>
-    <row r="65" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
         <v>31</v>
       </c>
@@ -4617,7 +4892,7 @@
       <c r="J65" s="28"/>
       <c r="K65" s="29"/>
       <c r="L65" s="37"/>
-      <c r="M65" s="39"/>
+      <c r="M65" s="98"/>
       <c r="N65" s="15"/>
       <c r="O65" s="28"/>
       <c r="P65" s="29"/>
@@ -4634,7 +4909,7 @@
       <c r="AR65" s="7"/>
       <c r="AS65" s="7"/>
     </row>
-    <row r="66" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A66" s="20" t="s">
         <v>32</v>
       </c>
@@ -4649,7 +4924,7 @@
       <c r="J66" s="28"/>
       <c r="K66" s="29"/>
       <c r="L66" s="37"/>
-      <c r="M66" s="39"/>
+      <c r="M66" s="98"/>
       <c r="N66" s="15"/>
       <c r="O66" s="28"/>
       <c r="P66" s="29"/>
@@ -4666,7 +4941,7 @@
       <c r="AR66" s="7"/>
       <c r="AS66" s="7"/>
     </row>
-    <row r="67" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A67" s="20" t="s">
         <v>33</v>
       </c>
@@ -4681,7 +4956,7 @@
       <c r="J67" s="28"/>
       <c r="K67" s="29"/>
       <c r="L67" s="37"/>
-      <c r="M67" s="39"/>
+      <c r="M67" s="98"/>
       <c r="N67" s="15"/>
       <c r="O67" s="28"/>
       <c r="P67" s="29"/>
@@ -4698,7 +4973,7 @@
       <c r="AR67" s="7"/>
       <c r="AS67" s="7"/>
     </row>
-    <row r="68" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A68" s="20" t="s">
         <v>34</v>
       </c>
@@ -4713,7 +4988,7 @@
       <c r="J68" s="28"/>
       <c r="K68" s="29"/>
       <c r="L68" s="37"/>
-      <c r="M68" s="39"/>
+      <c r="M68" s="98"/>
       <c r="N68" s="15"/>
       <c r="O68" s="28"/>
       <c r="P68" s="29"/>
@@ -4730,7 +5005,7 @@
       <c r="AR68" s="7"/>
       <c r="AS68" s="7"/>
     </row>
-    <row r="69" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A69" s="20" t="s">
         <v>35</v>
       </c>
@@ -4745,7 +5020,7 @@
       <c r="J69" s="28"/>
       <c r="K69" s="29"/>
       <c r="L69" s="37"/>
-      <c r="M69" s="39"/>
+      <c r="M69" s="98"/>
       <c r="N69" s="15"/>
       <c r="O69" s="28"/>
       <c r="P69" s="29"/>
@@ -4762,7 +5037,7 @@
       <c r="AR69" s="7"/>
       <c r="AS69" s="7"/>
     </row>
-    <row r="70" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A70" s="20" t="s">
         <v>36</v>
       </c>
@@ -4777,7 +5052,7 @@
       <c r="J70" s="28"/>
       <c r="K70" s="29"/>
       <c r="L70" s="37"/>
-      <c r="M70" s="39"/>
+      <c r="M70" s="98"/>
       <c r="N70" s="15"/>
       <c r="O70" s="28"/>
       <c r="P70" s="29"/>
@@ -4794,7 +5069,7 @@
       <c r="AR70" s="7"/>
       <c r="AS70" s="7"/>
     </row>
-    <row r="71" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A71" s="20" t="s">
         <v>37</v>
       </c>
@@ -4809,7 +5084,7 @@
       <c r="J71" s="28"/>
       <c r="K71" s="29"/>
       <c r="L71" s="37"/>
-      <c r="M71" s="39"/>
+      <c r="M71" s="98"/>
       <c r="N71" s="15"/>
       <c r="O71" s="28"/>
       <c r="P71" s="29"/>
@@ -4826,7 +5101,7 @@
       <c r="AR71" s="7"/>
       <c r="AS71" s="7"/>
     </row>
-    <row r="72" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A72" s="20" t="s">
         <v>38</v>
       </c>
@@ -4841,7 +5116,7 @@
       <c r="J72" s="28"/>
       <c r="K72" s="29"/>
       <c r="L72" s="37"/>
-      <c r="M72" s="39"/>
+      <c r="M72" s="98"/>
       <c r="N72" s="15"/>
       <c r="O72" s="28"/>
       <c r="P72" s="29"/>
@@ -4858,7 +5133,7 @@
       <c r="AR72" s="7"/>
       <c r="AS72" s="7"/>
     </row>
-    <row r="73" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A73" s="20" t="s">
         <v>39</v>
       </c>
@@ -4873,7 +5148,7 @@
       <c r="J73" s="28"/>
       <c r="K73" s="29"/>
       <c r="L73" s="37"/>
-      <c r="M73" s="39"/>
+      <c r="M73" s="98"/>
       <c r="N73" s="15"/>
       <c r="O73" s="28"/>
       <c r="P73" s="29"/>
@@ -4891,7 +5166,7 @@
       <c r="AS73" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:AS2331"/>
+  <autoFilter ref="A9:AS2331" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="A2:F4"/>
     <mergeCell ref="H8:L8"/>
@@ -5071,38 +5346,39 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Read-only column" error="TF84013: You cannot modify a field that is read-only or a work item that restricts updates to valid users based on current permissions." prompt="Read-only" sqref="P67:P68 K67:K68 U67:U68"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I11:I73 S12:S73 N12:N73 M11 R11">
+    <dataValidation operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Read-only column" error="TF84013: You cannot modify a field that is read-only or a work item that restricts updates to valid users based on current permissions." prompt="Read-only" sqref="P67:P68 K67:K68 U67:U68" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I11:I73 S12:S73 N12:N73 M11 R11" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Pendiente de Ejecución,Paso,Fallo,Bloqueado,No aplica"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B11:B73">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="B11:B73" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Alta,Media,Baja"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.51180555555555562" footer="0.51180555555555562"/>
   <pageSetup scale="27" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="44.42578125" customWidth="1"/>
-    <col min="5" max="5" width="43.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="44.44140625" customWidth="1"/>
+    <col min="5" max="5" width="43.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="42"/>
       <c r="B1" s="42"/>
       <c r="C1" s="42"/>
@@ -5112,7 +5388,7 @@
       <c r="G1" s="42"/>
       <c r="H1" s="42"/>
     </row>
-    <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>79</v>
       </c>
@@ -5138,7 +5414,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
@@ -5148,7 +5424,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="36" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>1</v>
       </c>
@@ -5159,48 +5435,48 @@
         <v>43753</v>
       </c>
       <c r="D4" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="E4" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="E4" s="26" t="s">
-        <v>198</v>
-      </c>
       <c r="F4" s="21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G4" s="21" t="s">
         <v>127</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="36" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>2</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C5" s="44">
         <v>43753</v>
       </c>
       <c r="D5" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="E5" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="F5" s="21" t="s">
         <v>202</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>203</v>
       </c>
       <c r="G5" s="21" t="s">
         <v>158</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="84" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <v>3</v>
       </c>
@@ -5211,22 +5487,22 @@
         <v>43753</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E6" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="F6" s="21" t="s">
         <v>204</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>205</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>127</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="36" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>4</v>
       </c>
@@ -5237,22 +5513,22 @@
         <v>43753</v>
       </c>
       <c r="D7" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="E7" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="F7" s="21" t="s">
         <v>207</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>208</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>158</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="36" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>5</v>
       </c>
@@ -5263,22 +5539,22 @@
         <v>43753</v>
       </c>
       <c r="D8" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="E8" s="21" t="s">
-        <v>210</v>
-      </c>
       <c r="F8" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G8" s="21" t="s">
         <v>127</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="36" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>6</v>
       </c>
@@ -5289,22 +5565,22 @@
         <v>43753</v>
       </c>
       <c r="D9" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="E9" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="E9" s="21" t="s">
-        <v>212</v>
-      </c>
       <c r="F9" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>158</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="36" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <v>7</v>
       </c>
@@ -5315,22 +5591,22 @@
         <v>43753</v>
       </c>
       <c r="D10" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>214</v>
-      </c>
       <c r="F10" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>158</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="36" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>8</v>
       </c>
@@ -5341,22 +5617,22 @@
         <v>43753</v>
       </c>
       <c r="D11" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="E11" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="E11" s="21" t="s">
-        <v>216</v>
-      </c>
       <c r="F11" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G11" s="21" t="s">
         <v>158</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="24" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>9</v>
       </c>
@@ -5367,22 +5643,22 @@
         <v>43753</v>
       </c>
       <c r="D12" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="E12" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="E12" s="21" t="s">
-        <v>219</v>
-      </c>
       <c r="F12" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G12" s="21" t="s">
         <v>158</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="36" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>10</v>
       </c>
@@ -5393,22 +5669,22 @@
         <v>43753</v>
       </c>
       <c r="D13" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="E13" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="E13" s="21" t="s">
-        <v>225</v>
-      </c>
       <c r="F13" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G13" s="21" t="s">
         <v>127</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <v>11</v>
       </c>
@@ -5420,7 +5696,7 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>12</v>
       </c>
@@ -5432,7 +5708,7 @@
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>13</v>
       </c>
@@ -5444,7 +5720,7 @@
       <c r="G16" s="21"/>
       <c r="H16" s="21"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <v>14</v>
       </c>
@@ -5456,7 +5732,7 @@
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <v>15</v>
       </c>
@@ -5470,13 +5746,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="G4:G18">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="G4:G18" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Alta,Media,Baja"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F18" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Bloqueante,Critico,Severo,Menor,Cosmetico"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H18" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Creado,En Desarrollo,En Prueba,Resuelto,Bloqueado,Cancelado,Cerrado"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5485,118 +5761,118 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G8" sqref="G8:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="55.140625" customWidth="1"/>
-    <col min="8" max="8" width="44.85546875" customWidth="1"/>
+    <col min="5" max="5" width="55.109375" customWidth="1"/>
+    <col min="8" max="8" width="44.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+    <row r="1" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="85"/>
-    </row>
-    <row r="2" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="80" t="s">
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="83"/>
+    </row>
+    <row r="2" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="86" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="80" t="s">
+      <c r="B2" s="87"/>
+      <c r="C2" s="86" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="82"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="80" t="s">
+      <c r="D2" s="88"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="82"/>
-      <c r="H2" s="81"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="87"/>
       <c r="I2" s="51"/>
       <c r="J2" s="51"/>
       <c r="K2" s="52"/>
       <c r="L2" s="46"/>
     </row>
-    <row r="3" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="83" t="s">
+    <row r="3" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="85"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="78" t="s">
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="83"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="79"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="53">
         <v>1</v>
       </c>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="84" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="76"/>
+      <c r="E4" s="85"/>
       <c r="F4" s="53">
         <v>3</v>
       </c>
-      <c r="G4" s="75" t="s">
+      <c r="G4" s="84" t="s">
         <v>94</v>
       </c>
-      <c r="H4" s="76"/>
+      <c r="H4" s="85"/>
       <c r="I4" s="45"/>
       <c r="J4" s="45"/>
       <c r="K4" s="45"/>
       <c r="L4" s="46"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="71"/>
-      <c r="B5" s="72"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="73"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="47">
         <v>2</v>
       </c>
-      <c r="D5" s="73" t="s">
+      <c r="D5" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="E5" s="74"/>
+      <c r="E5" s="79"/>
       <c r="F5" s="47">
         <v>4</v>
       </c>
-      <c r="G5" s="73" t="s">
+      <c r="G5" s="77" t="s">
         <v>95</v>
       </c>
-      <c r="H5" s="74"/>
+      <c r="H5" s="79"/>
       <c r="I5" s="45"/>
       <c r="J5" s="45"/>
       <c r="K5" s="45"/>
       <c r="L5" s="46"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="62"/>
       <c r="B6" s="63"/>
       <c r="C6" s="47"/>
@@ -5605,228 +5881,228 @@
       <c r="F6" s="47">
         <v>5</v>
       </c>
-      <c r="G6" s="73" t="s">
-        <v>226</v>
-      </c>
-      <c r="H6" s="74"/>
+      <c r="G6" s="77" t="s">
+        <v>225</v>
+      </c>
+      <c r="H6" s="79"/>
       <c r="I6" s="45"/>
       <c r="J6" s="45"/>
       <c r="K6" s="45"/>
       <c r="L6" s="46"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" s="46"/>
       <c r="C7" s="47"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="74"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="79"/>
       <c r="F7" s="47"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="74"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="79"/>
       <c r="I7" s="45"/>
       <c r="J7" s="45"/>
       <c r="K7" s="45"/>
       <c r="L7" s="46"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="77" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="74"/>
+      <c r="B8" s="79"/>
       <c r="C8" s="47">
         <v>6</v>
       </c>
-      <c r="D8" s="73" t="s">
+      <c r="D8" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="E8" s="74"/>
+      <c r="E8" s="79"/>
       <c r="F8" s="47">
         <v>7</v>
       </c>
-      <c r="G8" s="73" t="s">
+      <c r="G8" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="H8" s="74"/>
+      <c r="H8" s="79"/>
       <c r="I8" s="45"/>
       <c r="J8" s="45"/>
       <c r="K8" s="45"/>
       <c r="L8" s="46"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="47"/>
       <c r="B9" s="46"/>
       <c r="C9" s="47"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="79"/>
       <c r="F9" s="47"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="74"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="79"/>
       <c r="I9" s="45"/>
       <c r="J9" s="45"/>
       <c r="K9" s="45"/>
       <c r="L9" s="46"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="71" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="72"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="47">
         <v>8</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="77" t="s">
         <v>100</v>
       </c>
-      <c r="E10" s="74"/>
+      <c r="E10" s="79"/>
       <c r="F10" s="47">
         <v>10</v>
       </c>
-      <c r="G10" s="73" t="s">
+      <c r="G10" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="H10" s="74"/>
+      <c r="H10" s="79"/>
       <c r="I10" s="45"/>
       <c r="J10" s="45"/>
       <c r="K10" s="45"/>
       <c r="L10" s="46"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="71"/>
-      <c r="B11" s="72"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="73"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="47">
         <v>9</v>
       </c>
-      <c r="D11" s="73" t="s">
+      <c r="D11" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="E11" s="74"/>
+      <c r="E11" s="79"/>
       <c r="F11" s="47">
         <v>11</v>
       </c>
-      <c r="G11" s="73" t="s">
+      <c r="G11" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="H11" s="74"/>
+      <c r="H11" s="79"/>
       <c r="I11" s="45"/>
       <c r="J11" s="45"/>
       <c r="K11" s="45"/>
       <c r="L11" s="46"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="47"/>
       <c r="B12" s="46"/>
       <c r="C12" s="47"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="74"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="79"/>
       <c r="F12" s="47"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="74"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="79"/>
       <c r="I12" s="45"/>
       <c r="J12" s="45"/>
       <c r="K12" s="45"/>
       <c r="L12" s="46"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="71" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="73" t="s">
         <v>103</v>
       </c>
-      <c r="B13" s="72"/>
+      <c r="B13" s="74"/>
       <c r="C13" s="47">
         <v>12</v>
       </c>
-      <c r="D13" s="73" t="s">
+      <c r="D13" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="E13" s="74"/>
+      <c r="E13" s="79"/>
       <c r="F13" s="47">
         <v>14</v>
       </c>
-      <c r="G13" s="73" t="s">
+      <c r="G13" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="H13" s="74"/>
+      <c r="H13" s="79"/>
       <c r="I13" s="45"/>
       <c r="J13" s="45"/>
       <c r="K13" s="45"/>
       <c r="L13" s="46"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="71"/>
-      <c r="B14" s="72"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="73"/>
+      <c r="B14" s="74"/>
       <c r="C14" s="47"/>
       <c r="D14" s="57"/>
       <c r="E14" s="56"/>
       <c r="F14" s="47">
         <v>15</v>
       </c>
-      <c r="G14" s="73" t="s">
-        <v>196</v>
-      </c>
-      <c r="H14" s="74"/>
+      <c r="G14" s="77" t="s">
+        <v>195</v>
+      </c>
+      <c r="H14" s="79"/>
       <c r="I14" s="45"/>
       <c r="J14" s="45"/>
       <c r="K14" s="45"/>
       <c r="L14" s="46"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="71"/>
-      <c r="B15" s="72"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="73"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="47">
         <v>13</v>
       </c>
-      <c r="D15" s="73" t="s">
+      <c r="D15" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="E15" s="74"/>
+      <c r="E15" s="79"/>
       <c r="F15" s="47">
         <v>16</v>
       </c>
-      <c r="G15" s="73" t="s">
+      <c r="G15" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="H15" s="74"/>
+      <c r="H15" s="79"/>
       <c r="I15" s="45"/>
       <c r="J15" s="45"/>
       <c r="K15" s="45"/>
       <c r="L15" s="46"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="47"/>
       <c r="B16" s="46"/>
       <c r="C16" s="47"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="74"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="79"/>
       <c r="F16" s="47">
         <v>17</v>
       </c>
-      <c r="G16" s="73" t="s">
-        <v>194</v>
-      </c>
-      <c r="H16" s="74"/>
+      <c r="G16" s="77" t="s">
+        <v>193</v>
+      </c>
+      <c r="H16" s="79"/>
       <c r="I16" s="45"/>
       <c r="J16" s="45"/>
       <c r="K16" s="45"/>
       <c r="L16" s="46"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="47"/>
       <c r="B17" s="46"/>
       <c r="C17" s="47"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="74"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="79"/>
       <c r="F17" s="47">
         <v>18</v>
       </c>
-      <c r="G17" s="89" t="s">
-        <v>195</v>
-      </c>
-      <c r="H17" s="74"/>
+      <c r="G17" s="80" t="s">
+        <v>194</v>
+      </c>
+      <c r="H17" s="79"/>
       <c r="I17" s="47"/>
       <c r="J17" s="45"/>
       <c r="K17" s="45"/>
       <c r="L17" s="46"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
       <c r="B18" s="46"/>
       <c r="C18" s="47"/>
@@ -5838,48 +6114,48 @@
       <c r="K18" s="45"/>
       <c r="L18" s="46"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="71" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="B19" s="72"/>
+      <c r="B19" s="74"/>
       <c r="C19" s="47">
         <v>19</v>
       </c>
-      <c r="D19" s="73" t="s">
+      <c r="D19" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="74"/>
+      <c r="E19" s="79"/>
       <c r="F19" s="47">
         <v>21</v>
       </c>
-      <c r="G19" s="73" t="s">
+      <c r="G19" s="77" t="s">
         <v>111</v>
       </c>
-      <c r="H19" s="74"/>
+      <c r="H19" s="79"/>
       <c r="L19" s="46"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="71"/>
-      <c r="B20" s="72"/>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="73"/>
+      <c r="B20" s="74"/>
       <c r="C20" s="47">
         <v>20</v>
       </c>
-      <c r="D20" s="73" t="s">
+      <c r="D20" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="74"/>
+      <c r="E20" s="79"/>
       <c r="F20" s="47">
         <v>22</v>
       </c>
-      <c r="G20" s="73" t="s">
+      <c r="G20" s="77" t="s">
         <v>112</v>
       </c>
-      <c r="H20" s="74"/>
+      <c r="H20" s="79"/>
       <c r="I20" s="45"/>
       <c r="L20" s="46"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="47"/>
       <c r="B21" s="46"/>
       <c r="C21" s="47"/>
@@ -5893,7 +6169,7 @@
       <c r="K21" s="45"/>
       <c r="L21" s="46"/>
     </row>
-    <row r="22" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="48"/>
       <c r="B22" s="50"/>
       <c r="C22" s="48"/>
@@ -5907,173 +6183,173 @@
       <c r="K22" s="45"/>
       <c r="L22" s="46"/>
     </row>
-    <row r="23" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="83" t="s">
+    <row r="23" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="84"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="84"/>
-      <c r="K23" s="84"/>
-      <c r="L23" s="85"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="78" t="s">
+      <c r="B23" s="82"/>
+      <c r="C23" s="82"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="82"/>
+      <c r="G23" s="82"/>
+      <c r="H23" s="82"/>
+      <c r="I23" s="82"/>
+      <c r="J23" s="82"/>
+      <c r="K23" s="82"/>
+      <c r="L23" s="83"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="B24" s="79"/>
+      <c r="B24" s="72"/>
       <c r="C24" s="53">
         <v>23</v>
       </c>
-      <c r="D24" s="75" t="s">
-        <v>180</v>
-      </c>
-      <c r="E24" s="76"/>
+      <c r="D24" s="84" t="s">
+        <v>179</v>
+      </c>
+      <c r="E24" s="85"/>
       <c r="F24" s="53">
         <v>24</v>
       </c>
-      <c r="G24" s="75" t="s">
-        <v>181</v>
-      </c>
-      <c r="H24" s="76"/>
+      <c r="G24" s="84" t="s">
+        <v>180</v>
+      </c>
+      <c r="H24" s="85"/>
       <c r="I24" s="51"/>
       <c r="J24" s="51"/>
       <c r="K24" s="51"/>
       <c r="L24" s="52"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="71"/>
-      <c r="B25" s="72"/>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="73"/>
+      <c r="B25" s="74"/>
       <c r="C25" s="47"/>
       <c r="D25" s="45"/>
       <c r="E25" s="46"/>
       <c r="F25" s="47">
         <v>25</v>
       </c>
-      <c r="G25" s="73" t="s">
-        <v>182</v>
-      </c>
-      <c r="H25" s="74"/>
+      <c r="G25" s="77" t="s">
+        <v>181</v>
+      </c>
+      <c r="H25" s="79"/>
       <c r="I25" s="45"/>
       <c r="J25" s="45"/>
       <c r="K25" s="45"/>
       <c r="L25" s="46"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="71"/>
-      <c r="B26" s="72"/>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="73"/>
+      <c r="B26" s="74"/>
       <c r="C26" s="47"/>
       <c r="D26" s="45"/>
       <c r="E26" s="46"/>
       <c r="F26" s="47">
         <v>26</v>
       </c>
-      <c r="G26" s="73" t="s">
-        <v>183</v>
-      </c>
-      <c r="H26" s="74"/>
+      <c r="G26" s="77" t="s">
+        <v>182</v>
+      </c>
+      <c r="H26" s="79"/>
       <c r="I26" s="45"/>
       <c r="J26" s="45"/>
       <c r="K26" s="45"/>
       <c r="L26" s="46"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="71"/>
-      <c r="B27" s="72"/>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="73"/>
+      <c r="B27" s="74"/>
       <c r="C27" s="47"/>
       <c r="D27" s="45"/>
       <c r="E27" s="46"/>
       <c r="F27" s="47">
         <v>27</v>
       </c>
-      <c r="G27" s="73" t="s">
-        <v>184</v>
-      </c>
-      <c r="H27" s="74"/>
+      <c r="G27" s="77" t="s">
+        <v>183</v>
+      </c>
+      <c r="H27" s="79"/>
       <c r="I27" s="45"/>
       <c r="J27" s="45"/>
       <c r="K27" s="45"/>
       <c r="L27" s="46"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="71"/>
-      <c r="B28" s="72"/>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="73"/>
+      <c r="B28" s="74"/>
       <c r="C28" s="47"/>
       <c r="D28" s="45"/>
       <c r="E28" s="46"/>
       <c r="F28" s="47">
         <v>28</v>
       </c>
-      <c r="G28" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="H28" s="74"/>
+      <c r="G28" s="77" t="s">
+        <v>184</v>
+      </c>
+      <c r="H28" s="79"/>
       <c r="I28" s="45"/>
       <c r="J28" s="45"/>
       <c r="K28" s="45"/>
       <c r="L28" s="46"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="71"/>
-      <c r="B29" s="72"/>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="73"/>
+      <c r="B29" s="74"/>
       <c r="C29" s="45"/>
       <c r="D29" s="45"/>
       <c r="E29" s="46"/>
       <c r="F29" s="47">
         <v>29</v>
       </c>
-      <c r="G29" s="73" t="s">
-        <v>186</v>
-      </c>
-      <c r="H29" s="73"/>
+      <c r="G29" s="77" t="s">
+        <v>185</v>
+      </c>
+      <c r="H29" s="77"/>
       <c r="I29" s="47"/>
       <c r="J29" s="45"/>
       <c r="K29" s="45"/>
       <c r="L29" s="46"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="71"/>
-      <c r="B30" s="72"/>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="73"/>
+      <c r="B30" s="74"/>
       <c r="C30" s="45"/>
       <c r="D30" s="45"/>
       <c r="E30" s="45"/>
       <c r="F30" s="47">
         <v>30</v>
       </c>
-      <c r="G30" s="73" t="s">
-        <v>192</v>
-      </c>
-      <c r="H30" s="73"/>
+      <c r="G30" s="77" t="s">
+        <v>191</v>
+      </c>
+      <c r="H30" s="77"/>
       <c r="I30" s="47"/>
       <c r="J30" s="45"/>
       <c r="K30" s="45"/>
       <c r="L30" s="46"/>
     </row>
-    <row r="31" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="86"/>
-      <c r="B31" s="87"/>
+    <row r="31" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="75"/>
+      <c r="B31" s="76"/>
       <c r="C31" s="49"/>
       <c r="D31" s="49"/>
       <c r="E31" s="49"/>
       <c r="F31" s="48">
         <v>31</v>
       </c>
-      <c r="G31" s="88" t="s">
-        <v>193</v>
-      </c>
-      <c r="H31" s="88"/>
+      <c r="G31" s="78" t="s">
+        <v>192</v>
+      </c>
+      <c r="H31" s="78"/>
       <c r="I31" s="48"/>
       <c r="J31" s="49"/>
       <c r="K31" s="49"/>
       <c r="L31" s="50"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="47"/>
       <c r="B32" s="45"/>
       <c r="C32" s="45"/>
@@ -6087,7 +6363,7 @@
       <c r="K32" s="45"/>
       <c r="L32" s="46"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="47"/>
       <c r="B33" s="45"/>
       <c r="C33" s="45"/>
@@ -6101,7 +6377,7 @@
       <c r="K33" s="45"/>
       <c r="L33" s="46"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="47"/>
       <c r="B34" s="45"/>
       <c r="C34" s="45"/>
@@ -6115,7 +6391,7 @@
       <c r="K34" s="45"/>
       <c r="L34" s="46"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="47"/>
       <c r="B35" s="45"/>
       <c r="C35" s="45"/>
@@ -6129,7 +6405,7 @@
       <c r="K35" s="45"/>
       <c r="L35" s="46"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="47"/>
       <c r="B36" s="45"/>
       <c r="C36" s="45"/>
@@ -6143,7 +6419,7 @@
       <c r="K36" s="45"/>
       <c r="L36" s="46"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="47"/>
       <c r="B37" s="45"/>
       <c r="C37" s="45"/>
@@ -6157,7 +6433,7 @@
       <c r="K37" s="45"/>
       <c r="L37" s="46"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="47"/>
       <c r="B38" s="45"/>
       <c r="C38" s="45"/>
@@ -6171,7 +6447,7 @@
       <c r="K38" s="45"/>
       <c r="L38" s="46"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="47"/>
       <c r="B39" s="45"/>
       <c r="C39" s="45"/>
@@ -6185,7 +6461,7 @@
       <c r="K39" s="45"/>
       <c r="L39" s="46"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="47"/>
       <c r="B40" s="45"/>
       <c r="C40" s="45"/>
@@ -6199,7 +6475,7 @@
       <c r="K40" s="45"/>
       <c r="L40" s="46"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="47"/>
       <c r="B41" s="45"/>
       <c r="C41" s="45"/>
@@ -6213,7 +6489,7 @@
       <c r="K41" s="45"/>
       <c r="L41" s="46"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="47"/>
       <c r="B42" s="45"/>
       <c r="C42" s="45"/>
@@ -6227,7 +6503,7 @@
       <c r="K42" s="45"/>
       <c r="L42" s="46"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="47"/>
       <c r="B43" s="45"/>
       <c r="C43" s="45"/>
@@ -6241,7 +6517,7 @@
       <c r="K43" s="45"/>
       <c r="L43" s="46"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="47"/>
       <c r="B44" s="45"/>
       <c r="C44" s="45"/>
@@ -6255,7 +6531,7 @@
       <c r="K44" s="45"/>
       <c r="L44" s="46"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="47"/>
       <c r="B45" s="45"/>
       <c r="C45" s="45"/>
@@ -6269,7 +6545,7 @@
       <c r="K45" s="45"/>
       <c r="L45" s="46"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="47"/>
       <c r="B46" s="45"/>
       <c r="C46" s="45"/>
@@ -6283,7 +6559,7 @@
       <c r="K46" s="45"/>
       <c r="L46" s="46"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="47"/>
       <c r="B47" s="45"/>
       <c r="C47" s="45"/>
@@ -6297,7 +6573,7 @@
       <c r="K47" s="45"/>
       <c r="L47" s="46"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="47"/>
       <c r="B48" s="45"/>
       <c r="C48" s="45"/>
@@ -6311,7 +6587,7 @@
       <c r="K48" s="45"/>
       <c r="L48" s="46"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="47"/>
       <c r="B49" s="45"/>
       <c r="C49" s="45"/>
@@ -6325,7 +6601,7 @@
       <c r="K49" s="45"/>
       <c r="L49" s="46"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="47"/>
       <c r="B50" s="45"/>
       <c r="C50" s="45"/>
@@ -6339,7 +6615,7 @@
       <c r="K50" s="45"/>
       <c r="L50" s="46"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="47"/>
       <c r="B51" s="45"/>
       <c r="C51" s="45"/>
@@ -6353,7 +6629,7 @@
       <c r="K51" s="45"/>
       <c r="L51" s="46"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="47"/>
       <c r="B52" s="45"/>
       <c r="C52" s="45"/>
@@ -6367,7 +6643,7 @@
       <c r="K52" s="45"/>
       <c r="L52" s="46"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="47"/>
       <c r="B53" s="45"/>
       <c r="C53" s="45"/>
@@ -6381,7 +6657,7 @@
       <c r="K53" s="45"/>
       <c r="L53" s="46"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="47"/>
       <c r="B54" s="45"/>
       <c r="C54" s="45"/>
@@ -6395,7 +6671,7 @@
       <c r="K54" s="45"/>
       <c r="L54" s="46"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="47"/>
       <c r="B55" s="45"/>
       <c r="C55" s="45"/>
@@ -6409,7 +6685,7 @@
       <c r="K55" s="45"/>
       <c r="L55" s="46"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="47"/>
       <c r="B56" s="45"/>
       <c r="C56" s="45"/>
@@ -6423,7 +6699,7 @@
       <c r="K56" s="45"/>
       <c r="L56" s="46"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="47"/>
       <c r="B57" s="45"/>
       <c r="C57" s="45"/>
@@ -6437,7 +6713,7 @@
       <c r="K57" s="45"/>
       <c r="L57" s="46"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="47"/>
       <c r="B58" s="45"/>
       <c r="C58" s="45"/>
@@ -6451,7 +6727,7 @@
       <c r="K58" s="45"/>
       <c r="L58" s="46"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="47"/>
       <c r="B59" s="45"/>
       <c r="C59" s="45"/>
@@ -6465,7 +6741,7 @@
       <c r="K59" s="45"/>
       <c r="L59" s="46"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="47"/>
       <c r="B60" s="45"/>
       <c r="C60" s="45"/>
@@ -6479,7 +6755,7 @@
       <c r="K60" s="45"/>
       <c r="L60" s="46"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="47"/>
       <c r="B61" s="45"/>
       <c r="C61" s="45"/>
@@ -6493,7 +6769,7 @@
       <c r="K61" s="45"/>
       <c r="L61" s="46"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="47"/>
       <c r="B62" s="45"/>
       <c r="C62" s="45"/>
@@ -6507,7 +6783,7 @@
       <c r="K62" s="45"/>
       <c r="L62" s="46"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="47"/>
       <c r="B63" s="45"/>
       <c r="C63" s="45"/>
@@ -6521,7 +6797,7 @@
       <c r="K63" s="45"/>
       <c r="L63" s="46"/>
     </row>
-    <row r="64" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="48"/>
       <c r="B64" s="49"/>
       <c r="C64" s="49"/>
@@ -6537,26 +6813,19 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="A24:B31"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="A4:B5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
@@ -6573,21 +6842,28 @@
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="A10:B11"/>
+    <mergeCell ref="A4:B5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A24:B31"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="D24:E24"/>
     <mergeCell ref="A13:B15"/>
     <mergeCell ref="A19:B20"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -6603,15 +6879,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9EE5A02A2A6DC45B45E782DFEFDA45E" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7657f0a98c495c38e0a3edb0de0bfed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c79c8594d4fa4c9fd200c91a62336472" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -6737,6 +7004,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA349A94-BB86-4E02-9DFC-BCF7626CFB19}">
   <ds:schemaRefs>
@@ -6748,14 +7024,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6771,4 +7039,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>